<commit_message>
Update 1. .xlsx edited & .csv deleted
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A393D7C-8699-4E5C-BB6B-485A5A517663}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6230F51-E0E5-4B82-B6C0-EE73BF44ABA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,15 +52,6 @@
     <t>Итого, руб.</t>
   </si>
   <si>
-    <t>общая сумма графы "Итого"</t>
-  </si>
-  <si>
-    <t>средняя площадь</t>
-  </si>
-  <si>
-    <t>максимальная сумма к оплате</t>
-  </si>
-  <si>
     <t>Абделазиз</t>
   </si>
   <si>
@@ -172,7 +163,16 @@
     <t>Просрочка, дней</t>
   </si>
   <si>
-    <t>максимальный срок просрочки</t>
+    <t>общая сумма графы "Итого", руб.</t>
+  </si>
+  <si>
+    <t>средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>максимальный срок просрочки, дней</t>
+  </si>
+  <si>
+    <t>максимальная сумма к оплате, руб.</t>
   </si>
 </sst>
 </file>
@@ -505,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,6 +530,16 @@
       <c r="A1" s="1">
         <v>112</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -554,7 +564,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -571,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <f>SUM(70,-PRODUCT(SUM(A3,-1),0.5))</f>
@@ -614,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ref="C4:C38" si="0">SUM(70,-PRODUCT(SUM(A4,-1),0.5))</f>
@@ -657,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
@@ -700,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
@@ -743,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
@@ -786,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
@@ -829,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
@@ -872,7 +882,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
@@ -915,7 +925,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
@@ -958,7 +968,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
@@ -1001,7 +1011,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
@@ -1044,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
@@ -1087,7 +1097,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
@@ -1130,7 +1140,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
@@ -1173,7 +1183,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
@@ -1216,7 +1226,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
@@ -1259,7 +1269,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
@@ -1302,7 +1312,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
@@ -1345,7 +1355,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
@@ -1388,7 +1398,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
@@ -1431,7 +1441,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
@@ -1474,7 +1484,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
@@ -1517,7 +1527,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
@@ -1560,7 +1570,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
@@ -1603,7 +1613,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
@@ -1646,7 +1656,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
@@ -1689,7 +1699,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
@@ -1732,7 +1742,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
@@ -1775,7 +1785,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
@@ -1818,7 +1828,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
@@ -1861,7 +1871,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
@@ -1904,7 +1914,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
@@ -1947,7 +1957,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="0"/>
@@ -1990,7 +2000,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="0"/>
@@ -2033,7 +2043,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="0"/>
@@ -2076,7 +2086,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="0"/>
@@ -2114,41 +2124,136 @@
         <v>3504.0000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43">
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="1">
         <f>TRUNC(SUM(K3:K38))</f>
         <v>262315</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="1">
         <f>AVERAGE(C3:C38)</f>
         <v>61.25</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="1">
         <f>MAX(H3:H38)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="1">
         <f>MAX(K3:K38)</f>
         <v>8624.0000000000018</v>
       </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update 2. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6230F51-E0E5-4B82-B6C0-EE73BF44ABA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A50C21-7B53-4C76-91DD-D17B276A635C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,9 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -527,7 +525,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1" s="4">
         <v>112</v>
       </c>
       <c r="B1" s="1"/>

</xml_diff>

<commit_message>
Update 3. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A50C21-7B53-4C76-91DD-D17B276A635C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C792CDC3-0505-4EA5-81EE-836521B33890}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,15 +215,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,7 +506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -525,19 +526,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4">
+      <c r="A1" s="2">
         <v>112</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -575,21 +576,21 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
         <f>SUM(70,-PRODUCT(SUM(A3,-1),0.5))</f>
         <v>70</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <f>IF(A3&lt;33, $A$1*1.1,$A$1*0.55)</f>
         <v>123.20000000000002</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <f>PRODUCT(C3,D3)</f>
         <v>8624.0000000000018</v>
       </c>
@@ -600,39 +601,39 @@
       <c r="G3" s="3">
         <v>44805</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <f>IF(SUM(G3,-F3)&lt;0,0,SUM(G3,-F3))</f>
         <v>0</v>
       </c>
-      <c r="I3" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="I3" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J3" s="2">
         <f>PRODUCT(H3,I3)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
         <f>SUM(E3,J3)</f>
         <v>8624.0000000000018</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <f t="shared" ref="C4:C38" si="0">SUM(70,-PRODUCT(SUM(A4,-1),0.5))</f>
         <v>69.5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <f t="shared" ref="D4:D38" si="1">IF(A4&lt;33, $A$1*1.1,$A$1*0.55)</f>
         <v>123.20000000000002</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E38" si="2">PRODUCT(C4,D4)</f>
         <v>8562.4000000000015</v>
       </c>
@@ -643,39 +644,39 @@
       <c r="G4" s="3">
         <v>44806</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <f t="shared" ref="H4:H38" si="3">IF(SUM(G4,-F4)&lt;0,0,SUM(G4,-F4))</f>
         <v>0</v>
       </c>
-      <c r="I4" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="I4" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J4" s="2">
         <f t="shared" ref="J4:J38" si="4">PRODUCT(H4,I4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="2">
         <f t="shared" ref="K4:K38" si="5">SUM(E4,J4)</f>
         <v>8562.4000000000015</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="2"/>
         <v>8500.8000000000011</v>
       </c>
@@ -686,39 +687,39 @@
       <c r="G5" s="3">
         <v>44807</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I5" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="I5" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
         <f t="shared" si="5"/>
         <v>8500.8000000000011</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>68.5</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="2"/>
         <v>8439.2000000000007</v>
       </c>
@@ -729,39 +730,39 @@
       <c r="G6" s="3">
         <v>44808</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I6" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="I6" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J6" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="2">
         <f t="shared" si="5"/>
         <v>8439.2000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E7" s="2">
         <f t="shared" si="2"/>
         <v>8377.6</v>
       </c>
@@ -772,39 +773,39 @@
       <c r="G7" s="3">
         <v>44809</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I7" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I7" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J7" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="2">
         <f t="shared" si="5"/>
         <v>8377.6</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>67.5</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E8" s="2">
         <f t="shared" si="2"/>
         <v>8316.0000000000018</v>
       </c>
@@ -815,39 +816,39 @@
       <c r="G8" s="3">
         <v>44810</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I8" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="I8" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="2">
         <f t="shared" si="5"/>
         <v>8316.0000000000018</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="2"/>
         <v>8254.4000000000015</v>
       </c>
@@ -858,39 +859,39 @@
       <c r="G9" s="3">
         <v>44811</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I9" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="I9" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J9" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="2">
         <f t="shared" si="5"/>
         <v>8254.4000000000015</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>66.5</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E10" s="2">
         <f t="shared" si="2"/>
         <v>8192.8000000000011</v>
       </c>
@@ -901,39 +902,39 @@
       <c r="G10" s="3">
         <v>44812</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I10" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="I10" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J10" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
         <f t="shared" si="5"/>
         <v>8192.8000000000011</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E11" s="2">
         <f t="shared" si="2"/>
         <v>8131.2000000000007</v>
       </c>
@@ -944,39 +945,39 @@
       <c r="G11" s="3">
         <v>44813</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I11" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="I11" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
         <f t="shared" si="5"/>
         <v>8131.2000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>65.5</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E12" s="2">
         <f t="shared" si="2"/>
         <v>8069.6000000000013</v>
       </c>
@@ -987,39 +988,39 @@
       <c r="G12" s="3">
         <v>44814</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I12" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="I12" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="K12" s="2">
         <f t="shared" si="5"/>
         <v>8079.6000000000013</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E13" s="2">
         <f t="shared" si="2"/>
         <v>8008.0000000000009</v>
       </c>
@@ -1030,39 +1031,39 @@
       <c r="G13" s="3">
         <v>44815</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I13" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="I13" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J13" s="2">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="2">
         <f t="shared" si="5"/>
         <v>8028.0000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>64.5</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E14" s="2">
         <f t="shared" si="2"/>
         <v>7946.4000000000015</v>
       </c>
@@ -1073,39 +1074,39 @@
       <c r="G14" s="3">
         <v>44816</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I14" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="I14" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J14" s="2">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
         <f t="shared" si="5"/>
         <v>7976.4000000000015</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E15" s="2">
         <f t="shared" si="2"/>
         <v>7884.8000000000011</v>
       </c>
@@ -1116,39 +1117,39 @@
       <c r="G15" s="3">
         <v>44817</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="I15" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J15" s="1">
+      <c r="I15" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J15" s="2">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2">
         <f t="shared" si="5"/>
         <v>7924.8000000000011</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>63.5</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E16" s="2">
         <f t="shared" si="2"/>
         <v>7823.2000000000007</v>
       </c>
@@ -1159,39 +1160,39 @@
       <c r="G16" s="3">
         <v>44818</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I16" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="I16" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J16" s="2">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2">
         <f t="shared" si="5"/>
         <v>7873.2000000000007</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="D17" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
         <v>7761.6000000000013</v>
       </c>
@@ -1202,39 +1203,39 @@
       <c r="G17" s="3">
         <v>44819</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="I17" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="I17" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J17" s="2">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="2">
         <f t="shared" si="5"/>
         <v>7821.6000000000013</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E18" s="2">
         <f t="shared" si="2"/>
         <v>7700.0000000000009</v>
       </c>
@@ -1245,39 +1246,39 @@
       <c r="G18" s="3">
         <v>44820</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="I18" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="I18" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J18" s="2">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="2">
         <f t="shared" si="5"/>
         <v>7770.0000000000009</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="D19" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="D19" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E19" s="2">
         <f t="shared" si="2"/>
         <v>7638.4000000000015</v>
       </c>
@@ -1288,39 +1289,39 @@
       <c r="G19" s="3">
         <v>44821</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="I19" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J19" s="1">
+      <c r="I19" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J19" s="2">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="2">
         <f t="shared" si="5"/>
         <v>7718.4000000000015</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>61.5</v>
       </c>
-      <c r="D20" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="D20" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E20" s="2">
         <f t="shared" si="2"/>
         <v>7576.8000000000011</v>
       </c>
@@ -1331,39 +1332,39 @@
       <c r="G20" s="3">
         <v>44822</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I20" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J20" s="1">
+      <c r="I20" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J20" s="2">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="2">
         <f t="shared" si="5"/>
         <v>7666.8000000000011</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="D21" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D21" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E21" s="2">
         <f t="shared" si="2"/>
         <v>7515.2000000000007</v>
       </c>
@@ -1374,39 +1375,39 @@
       <c r="G21" s="3">
         <v>44823</v>
       </c>
-      <c r="H21" s="1">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="I21" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J21" s="1">
+      <c r="H21" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I21" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J21" s="2">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="2">
         <f t="shared" si="5"/>
         <v>7615.2000000000007</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>60.5</v>
       </c>
-      <c r="D22" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E22" s="2">
         <f t="shared" si="2"/>
         <v>7453.6000000000013</v>
       </c>
@@ -1417,39 +1418,39 @@
       <c r="G22" s="3">
         <v>44824</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="2">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="I22" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J22" s="1">
+      <c r="I22" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J22" s="2">
         <f t="shared" si="4"/>
         <v>110</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="2">
         <f t="shared" si="5"/>
         <v>7563.6000000000013</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="D23" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D23" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E23" s="2">
         <f t="shared" si="2"/>
         <v>7392.0000000000009</v>
       </c>
@@ -1460,39 +1461,39 @@
       <c r="G23" s="3">
         <v>44825</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="2">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="I23" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="I23" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J23" s="2">
         <f t="shared" si="4"/>
         <v>120</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="2">
         <f t="shared" si="5"/>
         <v>7512.0000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>59.5</v>
       </c>
-      <c r="D24" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="D24" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E24" s="2">
         <f t="shared" si="2"/>
         <v>7330.4000000000015</v>
       </c>
@@ -1503,39 +1504,39 @@
       <c r="G24" s="3">
         <v>44826</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="2">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="I24" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J24" s="1">
+      <c r="I24" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J24" s="2">
         <f t="shared" si="4"/>
         <v>130</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="2">
         <f t="shared" si="5"/>
         <v>7460.4000000000015</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="D25" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D25" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E25" s="2">
         <f t="shared" si="2"/>
         <v>7268.8000000000011</v>
       </c>
@@ -1546,39 +1547,39 @@
       <c r="G25" s="3">
         <v>44827</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="I25" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="I25" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J25" s="2">
         <f t="shared" si="4"/>
         <v>140</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="2">
         <f t="shared" si="5"/>
         <v>7408.8000000000011</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>58.5</v>
       </c>
-      <c r="D26" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="D26" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E26" s="2">
         <f t="shared" si="2"/>
         <v>7207.2000000000007</v>
       </c>
@@ -1589,39 +1590,39 @@
       <c r="G26" s="3">
         <v>44828</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="2">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="I26" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="I26" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J26" s="2">
         <f t="shared" si="4"/>
         <v>150</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="2">
         <f t="shared" si="5"/>
         <v>7357.2000000000007</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="D27" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="D27" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E27" s="2">
         <f t="shared" si="2"/>
         <v>7145.6000000000013</v>
       </c>
@@ -1632,39 +1633,39 @@
       <c r="G27" s="3">
         <v>44829</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="2">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="I27" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J27" s="1">
+      <c r="I27" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J27" s="2">
         <f t="shared" si="4"/>
         <v>160</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="2">
         <f t="shared" si="5"/>
         <v>7305.6000000000013</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>57.5</v>
       </c>
-      <c r="D28" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="D28" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E28" s="2">
         <f t="shared" si="2"/>
         <v>7084.0000000000009</v>
       </c>
@@ -1675,39 +1676,39 @@
       <c r="G28" s="3">
         <v>44830</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="2">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="I28" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="I28" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J28" s="2">
         <f t="shared" si="4"/>
         <v>170</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="2">
         <f t="shared" si="5"/>
         <v>7254.0000000000009</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="D29" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="D29" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E29" s="2">
         <f t="shared" si="2"/>
         <v>7022.4000000000005</v>
       </c>
@@ -1718,39 +1719,39 @@
       <c r="G29" s="3">
         <v>44831</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="2">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="I29" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J29" s="1">
+      <c r="I29" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J29" s="2">
         <f t="shared" si="4"/>
         <v>180</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="2">
         <f t="shared" si="5"/>
         <v>7202.4000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>56.5</v>
       </c>
-      <c r="D30" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D30" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E30" s="2">
         <f t="shared" si="2"/>
         <v>6960.8000000000011</v>
       </c>
@@ -1761,39 +1762,39 @@
       <c r="G30" s="3">
         <v>44832</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="2">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="I30" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J30" s="1">
+      <c r="I30" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J30" s="2">
         <f t="shared" si="4"/>
         <v>190</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="2">
         <f t="shared" si="5"/>
         <v>7150.8000000000011</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="D31" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="D31" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E31" s="2">
         <f t="shared" si="2"/>
         <v>6899.2000000000007</v>
       </c>
@@ -1804,39 +1805,39 @@
       <c r="G31" s="3">
         <v>44833</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="I31" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J31" s="1">
+      <c r="I31" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J31" s="2">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="2">
         <f t="shared" si="5"/>
         <v>7099.2000000000007</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>55.5</v>
       </c>
-      <c r="D32" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="D32" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E32" s="2">
         <f t="shared" si="2"/>
         <v>6837.6000000000013</v>
       </c>
@@ -1847,39 +1848,39 @@
       <c r="G32" s="3">
         <v>44834</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="2">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="I32" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J32" s="1">
+      <c r="I32" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J32" s="2">
         <f t="shared" si="4"/>
         <v>210</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="2">
         <f t="shared" si="5"/>
         <v>7047.6000000000013</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="D33" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="D33" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E33" s="2">
         <f t="shared" si="2"/>
         <v>6776.0000000000009</v>
       </c>
@@ -1890,39 +1891,39 @@
       <c r="G33" s="3">
         <v>44835</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="2">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="I33" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J33" s="1">
+      <c r="I33" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J33" s="2">
         <f t="shared" si="4"/>
         <v>220</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="2">
         <f t="shared" si="5"/>
         <v>6996.0000000000009</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>54.5</v>
       </c>
-      <c r="D34" s="1">
-        <f t="shared" si="1"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D34" s="2">
+        <f t="shared" si="1"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E34" s="2">
         <f t="shared" si="2"/>
         <v>6714.4000000000005</v>
       </c>
@@ -1933,39 +1934,39 @@
       <c r="G34" s="3">
         <v>44836</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="2">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="I34" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J34" s="1">
+      <c r="I34" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J34" s="2">
         <f t="shared" si="4"/>
         <v>230</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="2">
         <f t="shared" si="5"/>
         <v>6944.4000000000005</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="2">
         <f t="shared" si="1"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="2">
         <f t="shared" si="2"/>
         <v>3326.4000000000005</v>
       </c>
@@ -1976,39 +1977,39 @@
       <c r="G35" s="3">
         <v>44837</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="I35" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J35" s="1">
+      <c r="I35" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J35" s="2">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="2">
         <f t="shared" si="5"/>
         <v>3566.4000000000005</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>53.5</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="2">
         <f t="shared" si="1"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="2">
         <f t="shared" si="2"/>
         <v>3295.6000000000004</v>
       </c>
@@ -2019,39 +2020,39 @@
       <c r="G36" s="3">
         <v>44838</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="2">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="I36" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J36" s="1">
+      <c r="I36" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J36" s="2">
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="2">
         <f t="shared" si="5"/>
         <v>3545.6000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="2">
         <f t="shared" si="1"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="2">
         <f t="shared" si="2"/>
         <v>3264.8000000000006</v>
       </c>
@@ -2062,39 +2063,39 @@
       <c r="G37" s="3">
         <v>44839</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="2">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="I37" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J37" s="1">
+      <c r="I37" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J37" s="2">
         <f t="shared" si="4"/>
         <v>260</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="2">
         <f t="shared" si="5"/>
         <v>3524.8000000000006</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>52.5</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="2">
         <f t="shared" si="1"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2">
         <f t="shared" si="2"/>
         <v>3234.0000000000005</v>
       </c>
@@ -2105,19 +2106,19 @@
       <c r="G38" s="3">
         <v>44840</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="2">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="I38" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="J38" s="1">
+      <c r="I38" s="2">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J38" s="2">
         <f t="shared" si="4"/>
         <v>270</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="2">
         <f t="shared" si="5"/>
         <v>3504.0000000000005</v>
       </c>

</xml_diff>

<commit_message>
Update 6. fixed table1
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC62985-0C94-4459-8118-289FB1EE9FFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2C7746-D73D-4569-B4E1-10E280551580}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>№ Квартиры</t>
   </si>
   <si>
-    <t>Фамилия квартиросъемщика</t>
-  </si>
-  <si>
     <t>Площадь, кв.м.</t>
   </si>
   <si>
@@ -52,15 +49,6 @@
     <t>Итого, руб.</t>
   </si>
   <si>
-    <t>общая сумма графы "Итого"</t>
-  </si>
-  <si>
-    <t>средняя площадь</t>
-  </si>
-  <si>
-    <t>максимальная сумма к оплате</t>
-  </si>
-  <si>
     <t>Абделазиз</t>
   </si>
   <si>
@@ -172,7 +160,19 @@
     <t>Просрочка, дней</t>
   </si>
   <si>
-    <t>максимальный срок просрочки</t>
+    <t>Фамилия квартиросъёмщика</t>
+  </si>
+  <si>
+    <t>Максимальный срок просрочки, дней</t>
+  </si>
+  <si>
+    <t>Максимальная сумма к оплате, руб.</t>
+  </si>
+  <si>
+    <t>Средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>Общая сумма графы "Итого", руб.</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,50 +531,50 @@
       <c r="A1" s="1">
         <v>112</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <f>SUM(70,-PRODUCT(SUM(A3,-1),0.5))</f>
@@ -626,7 +626,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ref="C4:C38" si="0">SUM(70,-PRODUCT(SUM(A4,-1),0.5))</f>
@@ -670,7 +670,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
@@ -714,7 +714,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
@@ -758,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
@@ -802,7 +802,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
@@ -846,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
@@ -890,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
@@ -934,7 +934,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
@@ -978,7 +978,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
@@ -1022,7 +1022,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
@@ -1066,7 +1066,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
@@ -1110,7 +1110,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
@@ -1154,7 +1154,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
@@ -1198,7 +1198,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
@@ -1286,7 +1286,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
@@ -1330,7 +1330,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
@@ -1374,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
@@ -1418,7 +1418,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
@@ -1462,7 +1462,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
@@ -1506,7 +1506,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
@@ -1550,7 +1550,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
@@ -1594,7 +1594,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
@@ -1638,7 +1638,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
@@ -1682,7 +1682,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
@@ -1726,7 +1726,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
@@ -1770,7 +1770,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
@@ -1814,7 +1814,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
@@ -1858,7 +1858,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
@@ -1902,7 +1902,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
@@ -1946,7 +1946,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
@@ -1990,7 +1990,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="0"/>
@@ -2034,7 +2034,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="0"/>
@@ -2078,7 +2078,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="0"/>
@@ -2122,7 +2122,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="0"/>
@@ -2160,85 +2160,93 @@
         <v>3504.0000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="2">
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="1">
         <f>TRUNC(SUM(K3:K38))</f>
         <v>262315</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="1">
+        <f>AVERAGE(C3:C38)</f>
+        <v>61.25</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="1">
+        <f>MAX(H3:H38)</f>
+        <v>27</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="1">
+        <f>MAX(K3:K38)</f>
+        <v>8624.0000000000018</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="2">
-        <f>AVERAGE(C3:C38)</f>
-        <v>61.25</v>
-      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -2250,13 +2258,6 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="2">
-        <f>MAX(H3:H38)</f>
-        <v>27</v>
-      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -2268,13 +2269,6 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="2">
-        <f>MAX(K3:K38)</f>
-        <v>8624.0000000000018</v>
-      </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>

</xml_diff>

<commit_message>
Update 8. fixed table1
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitpr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FEFEAE-59F4-4783-80FD-411ACB802B1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8A2AAC-1AA2-4BB7-9F99-1EF611D76A79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,7 +172,7 @@
     <t>Максимальный срок просрочки, дней</t>
   </si>
   <si>
-    <t>Максимальная сумма просрочки, руб.</t>
+    <t>Максимальная сумма к оплате, руб.</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update 9. fixed table1
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8A2AAC-1AA2-4BB7-9F99-1EF611D76A79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB93E1-6E00-4250-BD2E-8A83A07D9D99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,11 +195,8 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,16 +224,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,1663 +480,1754 @@
       <c r="A1" s="2">
         <v>112</v>
       </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>70</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <f>1.1*A$1</f>
         <v>123.20000000000002</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <f t="shared" ref="E3:E38" si="0">C3*D3</f>
         <v>8624.0000000000018</v>
       </c>
-      <c r="F3" s="3">
-        <v>44813</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G3" s="4">
         <v>44805</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <f t="shared" ref="H3:H38" si="1">IF(F3&gt;=G3, 0, G3-F3)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="4">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="3">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3">
         <f t="shared" ref="J3:J38" si="2">H3*I3</f>
         <v>0</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="3">
         <f t="shared" ref="K3:K38" si="3">E3+J3</f>
         <v>8624.0000000000018</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <f t="shared" ref="A4:A38" si="4">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <f t="shared" ref="C4:C38" si="5">C3-0.5</f>
         <v>69.5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <f t="shared" ref="D4:D34" si="6">1.1*A$1</f>
         <v>123.20000000000002</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>8562.4000000000015</v>
       </c>
-      <c r="F4" s="3">
-        <f t="shared" ref="F4:F38" si="7">F3</f>
-        <v>44813</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4" s="4">
+        <f>F3</f>
+        <v>44813</v>
+      </c>
+      <c r="G4" s="4">
+        <f>G3+1</f>
         <v>44806</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="4">
-        <f t="shared" ref="I4:I38" si="8">I3</f>
-        <v>10</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I38" si="7">I3</f>
+        <v>10</v>
+      </c>
+      <c r="J4" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="3">
         <f t="shared" si="3"/>
         <v>8562.4000000000015</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <f t="shared" si="5"/>
         <v>69</v>
       </c>
-      <c r="D5" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>8500.8000000000011</v>
       </c>
-      <c r="F5" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="4">
+        <f t="shared" ref="F4:F38" si="8">F4</f>
+        <v>44813</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G38" si="9">G4+1</f>
         <v>44807</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="I5" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J5" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="3">
         <f t="shared" si="3"/>
         <v>8500.8000000000011</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <f t="shared" si="5"/>
         <v>68.5</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
         <v>8439.2000000000007</v>
       </c>
-      <c r="F6" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="9"/>
         <v>44808</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="I6" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J6" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="3">
         <f t="shared" si="3"/>
         <v>8439.2000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
-      <c r="D7" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>8377.6</v>
       </c>
-      <c r="F7" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="9"/>
         <v>44809</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="I7" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J7" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="3">
         <f t="shared" si="3"/>
         <v>8377.6</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <f t="shared" si="5"/>
         <v>67.5</v>
       </c>
-      <c r="D8" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>8316.0000000000018</v>
       </c>
-      <c r="F8" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="9"/>
         <v>44810</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="I8" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J8" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="3">
         <f t="shared" si="3"/>
         <v>8316.0000000000018</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <f t="shared" si="5"/>
         <v>67</v>
       </c>
-      <c r="D9" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>8254.4000000000015</v>
       </c>
-      <c r="F9" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="9"/>
         <v>44811</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="I9" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J9" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="3">
         <f t="shared" si="3"/>
         <v>8254.4000000000015</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <f t="shared" si="5"/>
         <v>66.5</v>
       </c>
-      <c r="D10" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
         <v>8192.8000000000011</v>
       </c>
-      <c r="F10" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="9"/>
         <v>44812</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="I10" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J10" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="3">
         <f t="shared" si="3"/>
         <v>8192.8000000000011</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <f t="shared" si="5"/>
         <v>66</v>
       </c>
-      <c r="D11" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="D11" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E11" s="3">
         <f t="shared" si="0"/>
         <v>8131.2000000000007</v>
       </c>
-      <c r="F11" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G11" s="3">
-        <v>44813</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="F11" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="9"/>
+        <v>44813</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="I11" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J11" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="3">
         <f t="shared" si="3"/>
         <v>8131.2000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="3">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <f t="shared" si="5"/>
         <v>65.5</v>
       </c>
-      <c r="D12" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E12" s="3">
         <f t="shared" si="0"/>
         <v>8069.6000000000013</v>
       </c>
-      <c r="F12" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="9"/>
         <v>44814</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I12" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J12" s="2">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="K12" s="2">
+      <c r="I12" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="3"/>
         <v>8079.6000000000013</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <f t="shared" si="5"/>
         <v>65</v>
       </c>
-      <c r="D13" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="0"/>
         <v>8008.0000000000009</v>
       </c>
-      <c r="F13" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F13" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="9"/>
         <v>44815</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I13" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="I13" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J13" s="3">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="3">
         <f t="shared" si="3"/>
         <v>8028.0000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <f t="shared" si="5"/>
         <v>64.5</v>
       </c>
-      <c r="D14" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E14" s="3">
         <f t="shared" si="0"/>
         <v>7946.4000000000015</v>
       </c>
-      <c r="F14" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F14" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="9"/>
         <v>44816</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I14" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="I14" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="3">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="3">
         <f t="shared" si="3"/>
         <v>7976.4000000000015</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <f t="shared" si="5"/>
         <v>64</v>
       </c>
-      <c r="D15" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="D15" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
         <v>7884.8000000000011</v>
       </c>
-      <c r="F15" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="F15" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I15" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="I15" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J15" s="3">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="3">
         <f t="shared" si="3"/>
         <v>7924.8000000000011</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <f t="shared" si="5"/>
         <v>63.5</v>
       </c>
-      <c r="D16" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E16" s="3">
         <f t="shared" si="0"/>
         <v>7823.2000000000007</v>
       </c>
-      <c r="F16" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F16" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="9"/>
         <v>44818</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I16" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="I16" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J16" s="3">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="3">
         <f t="shared" si="3"/>
         <v>7873.2000000000007</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <f t="shared" si="5"/>
         <v>63</v>
       </c>
-      <c r="D17" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="D17" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E17" s="3">
         <f t="shared" si="0"/>
         <v>7761.6000000000013</v>
       </c>
-      <c r="F17" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="F17" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="9"/>
         <v>44819</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I17" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="I17" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J17" s="3">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="3">
         <f t="shared" si="3"/>
         <v>7821.6000000000013</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <f t="shared" si="5"/>
         <v>62.5</v>
       </c>
-      <c r="D18" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="D18" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E18" s="3">
         <f t="shared" si="0"/>
         <v>7700.0000000000009</v>
       </c>
-      <c r="F18" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="F18" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="9"/>
         <v>44820</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="3">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I18" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="I18" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J18" s="3">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="3">
         <f t="shared" si="3"/>
         <v>7770.0000000000009</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <f t="shared" si="5"/>
         <v>62</v>
       </c>
-      <c r="D19" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D19" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E19" s="3">
         <f t="shared" si="0"/>
         <v>7638.4000000000015</v>
       </c>
-      <c r="F19" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F19" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="9"/>
         <v>44821</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I19" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="I19" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J19" s="3">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="3">
         <f t="shared" si="3"/>
         <v>7718.4000000000015</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <f t="shared" si="5"/>
         <v>61.5</v>
       </c>
-      <c r="D20" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D20" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E20" s="3">
         <f t="shared" si="0"/>
         <v>7576.8000000000011</v>
       </c>
-      <c r="F20" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="F20" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="9"/>
         <v>44822</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I20" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J20" s="2">
+      <c r="I20" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J20" s="3">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="3">
         <f t="shared" si="3"/>
         <v>7666.8000000000011</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
-      <c r="D21" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="D21" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E21" s="3">
         <f t="shared" si="0"/>
         <v>7515.2000000000007</v>
       </c>
-      <c r="F21" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="F21" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="9"/>
         <v>44823</v>
       </c>
-      <c r="H21" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J21" s="2">
+      <c r="H21" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J21" s="3">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="3">
         <f t="shared" si="3"/>
         <v>7615.2000000000007</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <f t="shared" si="5"/>
         <v>60.5</v>
       </c>
-      <c r="D22" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="D22" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E22" s="3">
         <f t="shared" si="0"/>
         <v>7453.6000000000013</v>
       </c>
-      <c r="F22" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="9"/>
         <v>44824</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I22" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J22" s="2">
+      <c r="I22" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J22" s="3">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="3">
         <f t="shared" si="3"/>
         <v>7563.6000000000013</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="D23" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D23" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E23" s="3">
         <f t="shared" si="0"/>
         <v>7392.0000000000009</v>
       </c>
-      <c r="F23" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G23" s="3">
+      <c r="F23" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="9"/>
         <v>44825</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I23" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J23" s="2">
+      <c r="I23" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J23" s="3">
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="3">
         <f t="shared" si="3"/>
         <v>7512.0000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <f t="shared" si="5"/>
         <v>59.5</v>
       </c>
-      <c r="D24" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E24" s="3">
         <f t="shared" si="0"/>
         <v>7330.4000000000015</v>
       </c>
-      <c r="F24" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="F24" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="9"/>
         <v>44826</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I24" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J24" s="2">
+      <c r="I24" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J24" s="3">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="3">
         <f t="shared" si="3"/>
         <v>7460.4000000000015</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <f t="shared" si="5"/>
         <v>59</v>
       </c>
-      <c r="D25" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E25" s="3">
         <f t="shared" si="0"/>
         <v>7268.8000000000011</v>
       </c>
-      <c r="F25" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G25" s="3">
+      <c r="F25" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="9"/>
         <v>44827</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I25" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J25" s="2">
+      <c r="I25" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J25" s="3">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="3">
         <f t="shared" si="3"/>
         <v>7408.8000000000011</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="3">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <f t="shared" si="5"/>
         <v>58.5</v>
       </c>
-      <c r="D26" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="D26" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E26" s="3">
         <f t="shared" si="0"/>
         <v>7207.2000000000007</v>
       </c>
-      <c r="F26" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G26" s="3">
+      <c r="F26" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="9"/>
         <v>44828</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I26" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J26" s="2">
+      <c r="I26" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J26" s="3">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="3">
         <f t="shared" si="3"/>
         <v>7357.2000000000007</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="3">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <f t="shared" si="5"/>
         <v>58</v>
       </c>
-      <c r="D27" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E27" s="2">
+      <c r="D27" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E27" s="3">
         <f t="shared" si="0"/>
         <v>7145.6000000000013</v>
       </c>
-      <c r="F27" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G27" s="3">
+      <c r="F27" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="9"/>
         <v>44829</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I27" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J27" s="2">
+      <c r="I27" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J27" s="3">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="3">
         <f t="shared" si="3"/>
         <v>7305.6000000000013</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="3">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="3">
         <f t="shared" si="5"/>
         <v>57.5</v>
       </c>
-      <c r="D28" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="D28" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E28" s="3">
         <f t="shared" si="0"/>
         <v>7084.0000000000009</v>
       </c>
-      <c r="F28" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G28" s="3">
+      <c r="F28" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="9"/>
         <v>44830</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I28" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J28" s="2">
+      <c r="I28" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J28" s="3">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="3">
         <f t="shared" si="3"/>
         <v>7254.0000000000009</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="3">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <f t="shared" si="5"/>
         <v>57</v>
       </c>
-      <c r="D29" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="D29" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E29" s="3">
         <f t="shared" si="0"/>
         <v>7022.4000000000005</v>
       </c>
-      <c r="F29" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G29" s="3">
+      <c r="F29" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="9"/>
         <v>44831</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I29" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J29" s="2">
+      <c r="I29" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J29" s="3">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="3">
         <f t="shared" si="3"/>
         <v>7202.4000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <f t="shared" si="5"/>
         <v>56.5</v>
       </c>
-      <c r="D30" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="D30" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E30" s="3">
         <f t="shared" si="0"/>
         <v>6960.8000000000011</v>
       </c>
-      <c r="F30" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G30" s="3">
+      <c r="F30" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G30" s="4">
+        <f t="shared" si="9"/>
         <v>44832</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="3">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I30" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J30" s="2">
+      <c r="I30" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J30" s="3">
         <f t="shared" si="2"/>
         <v>190</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="3">
         <f t="shared" si="3"/>
         <v>7150.8000000000011</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="3">
         <f t="shared" si="5"/>
         <v>56</v>
       </c>
-      <c r="D31" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E31" s="2">
+      <c r="D31" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E31" s="3">
         <f t="shared" si="0"/>
         <v>6899.2000000000007</v>
       </c>
-      <c r="F31" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="F31" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" si="9"/>
         <v>44833</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I31" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J31" s="2">
+      <c r="I31" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J31" s="3">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="3">
         <f t="shared" si="3"/>
         <v>7099.2000000000007</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="3">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <f t="shared" si="5"/>
         <v>55.5</v>
       </c>
-      <c r="D32" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="D32" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E32" s="3">
         <f t="shared" si="0"/>
         <v>6837.6000000000013</v>
       </c>
-      <c r="F32" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="F32" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" si="9"/>
         <v>44834</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="3">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I32" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J32" s="2">
+      <c r="I32" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J32" s="3">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="3">
         <f t="shared" si="3"/>
         <v>7047.6000000000013</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="3">
         <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="3">
         <f t="shared" si="5"/>
         <v>55</v>
       </c>
-      <c r="D33" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="D33" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E33" s="3">
         <f t="shared" si="0"/>
         <v>6776.0000000000009</v>
       </c>
-      <c r="F33" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G33" s="3">
+      <c r="F33" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="9"/>
         <v>44835</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="3">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I33" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J33" s="2">
+      <c r="I33" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J33" s="3">
         <f t="shared" si="2"/>
         <v>220</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="3">
         <f t="shared" si="3"/>
         <v>6996.0000000000009</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <f t="shared" si="5"/>
         <v>54.5</v>
       </c>
-      <c r="D34" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="D34" s="3">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E34" s="3">
         <f t="shared" si="0"/>
         <v>6714.4000000000005</v>
       </c>
-      <c r="F34" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G34" s="3">
+      <c r="F34" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" si="9"/>
         <v>44836</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I34" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J34" s="2">
+      <c r="I34" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J34" s="3">
         <f t="shared" si="2"/>
         <v>230</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="3">
         <f t="shared" si="3"/>
         <v>6944.4000000000005</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="3">
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="3">
         <f t="shared" si="5"/>
         <v>54</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="3">
         <f>0.55*A$1</f>
         <v>61.600000000000009</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="3">
         <f t="shared" si="0"/>
         <v>3326.4000000000005</v>
       </c>
-      <c r="F35" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G35" s="3">
+      <c r="F35" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" si="9"/>
         <v>44837</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I35" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J35" s="2">
+      <c r="I35" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J35" s="3">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="3">
         <f t="shared" si="3"/>
         <v>3566.4000000000005</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="3">
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="3">
         <f t="shared" si="5"/>
         <v>53.5</v>
       </c>
-      <c r="D36" s="2">
-        <f t="shared" ref="D36:D38" si="9">0.55*A$1</f>
+      <c r="D36" s="3">
+        <f t="shared" ref="D36:D38" si="10">0.55*A$1</f>
         <v>61.600000000000009</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="3">
         <f t="shared" si="0"/>
         <v>3295.6000000000004</v>
       </c>
-      <c r="F36" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G36" s="3">
+      <c r="F36" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" si="9"/>
         <v>44838</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="3">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I36" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J36" s="2">
+      <c r="I36" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J36" s="3">
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="3">
         <f t="shared" si="3"/>
         <v>3545.6000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="3">
         <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="3">
         <f t="shared" si="5"/>
         <v>53</v>
       </c>
-      <c r="D37" s="2">
-        <f t="shared" si="9"/>
+      <c r="D37" s="3">
+        <f t="shared" si="10"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="3">
         <f t="shared" si="0"/>
         <v>3264.8000000000006</v>
       </c>
-      <c r="F37" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G37" s="3">
+      <c r="F37" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G37" s="4">
+        <f t="shared" si="9"/>
         <v>44839</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I37" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J37" s="2">
+      <c r="I37" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J37" s="3">
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="3">
         <f t="shared" si="3"/>
         <v>3524.8000000000006</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="3">
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <f t="shared" si="5"/>
         <v>52.5</v>
       </c>
-      <c r="D38" s="2">
-        <f t="shared" si="9"/>
+      <c r="D38" s="3">
+        <f t="shared" si="10"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="3">
         <f t="shared" si="0"/>
         <v>3234.0000000000005</v>
       </c>
-      <c r="F38" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G38" s="3">
+      <c r="F38" s="4">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="G38" s="4">
+        <f t="shared" si="9"/>
         <v>44840</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="3">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I38" s="4">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="J38" s="2">
+      <c r="I38" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="J38" s="3">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="3">
         <f t="shared" si="3"/>
         <v>3504.0000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
       <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="5"/>
+      <c r="B40" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="3">
         <f>INT(SUM(K3:K38))</f>
         <v>262315</v>
       </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+      <c r="A41" s="5"/>
+      <c r="B41" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <f>AVERAGE(C3:C38)</f>
         <v>61.25</v>
       </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="5"/>
+      <c r="B42" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <f>MAX(H3:H38)</f>
         <v>27</v>
       </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
+      <c r="A43" s="5"/>
+      <c r="B43" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <f>MAX(J3, J38)</f>
         <v>270</v>
       </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.70000004768371604" right="0.70000004768371604" top="0.75" bottom="0.75" header="0.30000001192092901" footer="0.30000001192092901"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 11. Recheck table_1_112.xlsx
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08065C41-E24E-4AEE-997C-DEA9D8F0478C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D53DA5A-EF8B-499E-BA0B-2E9CB838F2E2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,6 +233,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -456,9 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -476,7 +475,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+      <c r="A1" s="5">
         <v>112</v>
       </c>
       <c r="B1" s="4"/>

</xml_diff>

<commit_message>
Update 12. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D53DA5A-EF8B-499E-BA0B-2E9CB838F2E2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF899261-002E-4D48-A47C-339DEA040E6E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -457,7 +457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -535,7 +537,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="2">
-        <f>1.1*A$1</f>
+        <f>IF(A3&lt;33, $A$1*1.1,$A$1*0.55)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="2">
@@ -549,35 +551,35 @@
         <v>44805</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H38" si="1">IF(F3&gt;=G3, 0, G3-F3)</f>
+        <f>IF(G3&lt;F3, 0, G3-F3)</f>
         <v>0</v>
       </c>
       <c r="I3" s="2">
         <v>10</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J38" si="2">H3*I3</f>
+        <f t="shared" ref="J3:J38" si="1">H3*I3</f>
         <v>0</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K38" si="3">E3+J3</f>
+        <f t="shared" ref="K3:K38" si="2">E3+J3</f>
         <v>8624.0000000000018</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A38" si="4">A3+1</f>
+        <f t="shared" ref="A4:A38" si="3">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C38" si="5">C3-0.5</f>
+        <f t="shared" ref="C4:C38" si="4">C3-0.5</f>
         <v>69.5</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D34" si="6">1.1*A$1</f>
+        <f t="shared" ref="D4:D38" si="5">IF(A4&lt;33, $A$1*1.1,$A$1*0.55)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="2">
@@ -593,7 +595,7 @@
         <v>44806</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H4:H38" si="6">IF(G4&lt;F4, 0, G4-F4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="2">
@@ -601,28 +603,28 @@
         <v>10</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8562.4000000000015</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="2">
@@ -638,7 +640,7 @@
         <v>44807</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I5" s="2">
@@ -646,28 +648,28 @@
         <v>10</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8500.8000000000011</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>68.5</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E6" s="2">
@@ -683,7 +685,7 @@
         <v>44808</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
@@ -691,28 +693,28 @@
         <v>10</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8439.2000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E7" s="2">
@@ -728,7 +730,7 @@
         <v>44809</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I7" s="2">
@@ -736,28 +738,28 @@
         <v>10</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8377.6</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E8" s="2">
@@ -773,7 +775,7 @@
         <v>44810</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I8" s="2">
@@ -781,28 +783,28 @@
         <v>10</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8316.0000000000018</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E9" s="2">
@@ -818,7 +820,7 @@
         <v>44811</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I9" s="2">
@@ -826,28 +828,28 @@
         <v>10</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8254.4000000000015</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>66.5</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E10" s="2">
@@ -863,7 +865,7 @@
         <v>44812</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I10" s="2">
@@ -871,28 +873,28 @@
         <v>10</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8192.8000000000011</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E11" s="2">
@@ -908,7 +910,7 @@
         <v>44813</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I11" s="2">
@@ -916,28 +918,28 @@
         <v>10</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8131.2000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>65.5</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E12" s="2">
@@ -953,7 +955,7 @@
         <v>44814</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I12" s="2">
@@ -961,28 +963,28 @@
         <v>10</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8079.6000000000013</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E13" s="2">
@@ -998,7 +1000,7 @@
         <v>44815</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I13" s="2">
@@ -1006,28 +1008,28 @@
         <v>10</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8028.0000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>64.5</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E14" s="2">
@@ -1043,7 +1045,7 @@
         <v>44816</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I14" s="2">
@@ -1051,28 +1053,28 @@
         <v>10</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7976.4000000000015</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E15" s="2">
@@ -1088,7 +1090,7 @@
         <v>44817</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I15" s="2">
@@ -1096,28 +1098,28 @@
         <v>10</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7924.8000000000011</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63.5</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E16" s="2">
@@ -1133,7 +1135,7 @@
         <v>44818</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I16" s="2">
@@ -1141,28 +1143,28 @@
         <v>10</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7873.2000000000007</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E17" s="2">
@@ -1178,7 +1180,7 @@
         <v>44819</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I17" s="2">
@@ -1186,28 +1188,28 @@
         <v>10</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7821.6000000000013</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E18" s="2">
@@ -1223,7 +1225,7 @@
         <v>44820</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I18" s="2">
@@ -1231,28 +1233,28 @@
         <v>10</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7770.0000000000009</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E19" s="2">
@@ -1268,7 +1270,7 @@
         <v>44821</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="I19" s="2">
@@ -1276,28 +1278,28 @@
         <v>10</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7718.4000000000015</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61.5</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E20" s="2">
@@ -1313,7 +1315,7 @@
         <v>44822</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="I20" s="2">
@@ -1321,28 +1323,28 @@
         <v>10</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7666.8000000000011</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E21" s="2">
@@ -1358,7 +1360,7 @@
         <v>44823</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="I21" s="2">
@@ -1366,28 +1368,28 @@
         <v>10</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7615.2000000000007</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>60.5</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E22" s="2">
@@ -1403,7 +1405,7 @@
         <v>44824</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="I22" s="2">
@@ -1411,28 +1413,28 @@
         <v>10</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7563.6000000000013</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E23" s="2">
@@ -1448,7 +1450,7 @@
         <v>44825</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="I23" s="2">
@@ -1456,28 +1458,28 @@
         <v>10</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7512.0000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>59.5</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E24" s="2">
@@ -1493,7 +1495,7 @@
         <v>44826</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="I24" s="2">
@@ -1501,28 +1503,28 @@
         <v>10</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7460.4000000000015</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E25" s="2">
@@ -1538,7 +1540,7 @@
         <v>44827</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="I25" s="2">
@@ -1546,28 +1548,28 @@
         <v>10</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7408.8000000000011</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>58.5</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E26" s="2">
@@ -1583,7 +1585,7 @@
         <v>44828</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I26" s="2">
@@ -1591,28 +1593,28 @@
         <v>10</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7357.2000000000007</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E27" s="2">
@@ -1628,7 +1630,7 @@
         <v>44829</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="I27" s="2">
@@ -1636,28 +1638,28 @@
         <v>10</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7305.6000000000013</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>57.5</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E28" s="2">
@@ -1673,7 +1675,7 @@
         <v>44830</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="I28" s="2">
@@ -1681,28 +1683,28 @@
         <v>10</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>170</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7254.0000000000009</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E29" s="2">
@@ -1718,7 +1720,7 @@
         <v>44831</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="I29" s="2">
@@ -1726,28 +1728,28 @@
         <v>10</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7202.4000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>56.5</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E30" s="2">
@@ -1763,7 +1765,7 @@
         <v>44832</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="I30" s="2">
@@ -1771,28 +1773,28 @@
         <v>10</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>190</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7150.8000000000011</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E31" s="2">
@@ -1808,7 +1810,7 @@
         <v>44833</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I31" s="2">
@@ -1816,28 +1818,28 @@
         <v>10</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7099.2000000000007</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>55.5</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E32" s="2">
@@ -1853,7 +1855,7 @@
         <v>44834</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="I32" s="2">
@@ -1861,28 +1863,28 @@
         <v>10</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7047.6000000000013</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E33" s="2">
@@ -1898,7 +1900,7 @@
         <v>44835</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="I33" s="2">
@@ -1906,28 +1908,28 @@
         <v>10</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6996.0000000000009</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>54.5</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E34" s="2">
@@ -1943,7 +1945,7 @@
         <v>44836</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="I34" s="2">
@@ -1951,28 +1953,28 @@
         <v>10</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>230</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6944.4000000000005</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="D35" s="2">
-        <f>0.55*A$1</f>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E35" s="2">
@@ -1988,7 +1990,7 @@
         <v>44837</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="I35" s="2">
@@ -1996,28 +1998,28 @@
         <v>10</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3566.4000000000005</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>53.5</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" ref="D36:D38" si="10">0.55*A$1</f>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E36" s="2">
@@ -2033,7 +2035,7 @@
         <v>44838</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="I36" s="2">
@@ -2041,28 +2043,28 @@
         <v>10</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3545.6000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E37" s="2">
@@ -2078,7 +2080,7 @@
         <v>44839</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="I37" s="2">
@@ -2086,28 +2088,28 @@
         <v>10</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>260</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3524.8000000000006</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E38" s="2">
@@ -2123,7 +2125,7 @@
         <v>44840</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="I38" s="2">
@@ -2131,11 +2133,11 @@
         <v>10</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>270</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3504.0000000000005</v>
       </c>
     </row>
@@ -2212,8 +2214,8 @@
         <v>50</v>
       </c>
       <c r="C43" s="2">
-        <f>MAX(J3, J38)</f>
-        <v>270</v>
+        <f>MAX(K3:K38)</f>
+        <v>8624.0000000000018</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>

</xml_diff>

<commit_message>
Update 13. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF899261-002E-4D48-A47C-339DEA040E6E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0391CD-B0C5-4A56-8834-4F7E5AB7A604}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +466,7 @@
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
@@ -537,7 +537,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="2">
-        <f>IF(A3&lt;33, $A$1*1.1,$A$1*0.55)</f>
+        <f>1.1*A1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="2">
@@ -551,7 +551,6 @@
         <v>44805</v>
       </c>
       <c r="H3" s="2">
-        <f>IF(G3&lt;F3, 0, G3-F3)</f>
         <v>0</v>
       </c>
       <c r="I3" s="2">
@@ -579,7 +578,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D38" si="5">IF(A4&lt;33, $A$1*1.1,$A$1*0.55)</f>
+        <f>IF(A4&lt;33, D$3,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="2">
@@ -595,11 +594,11 @@
         <v>44806</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H38" si="6">IF(G4&lt;F4, 0, G4-F4)</f>
+        <f>IF(G4&lt;=F4, H3, H3+1)</f>
         <v>0</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I38" si="7">I3</f>
+        <f t="shared" ref="I4:I38" si="5">I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="2">
@@ -624,7 +623,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D5:D38" si="6">IF(A5&lt;33, D$3,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="2">
@@ -632,19 +631,19 @@
         <v>8500.8000000000011</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F38" si="8">F4</f>
+        <f t="shared" ref="F5:F38" si="7">F4</f>
         <v>44813</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G38" si="9">G4+1</f>
+        <f t="shared" ref="G5:G38" si="8">G4+1</f>
         <v>44807</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H5:H38" si="9">IF(G5&lt;=F5, H4, H4+1)</f>
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J5" s="2">
@@ -669,7 +668,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E6" s="2">
@@ -677,19 +676,19 @@
         <v>8439.2000000000007</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44808</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J6" s="2">
@@ -714,7 +713,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E7" s="2">
@@ -722,19 +721,19 @@
         <v>8377.6</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44809</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J7" s="2">
@@ -759,7 +758,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E8" s="2">
@@ -767,19 +766,19 @@
         <v>8316.0000000000018</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44810</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J8" s="2">
@@ -804,7 +803,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E9" s="2">
@@ -812,19 +811,19 @@
         <v>8254.4000000000015</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44811</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J9" s="2">
@@ -849,7 +848,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E10" s="2">
@@ -857,19 +856,19 @@
         <v>8192.8000000000011</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44812</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J10" s="2">
@@ -894,7 +893,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E11" s="2">
@@ -902,19 +901,19 @@
         <v>8131.2000000000007</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J11" s="2">
@@ -939,7 +938,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E12" s="2">
@@ -947,19 +946,19 @@
         <v>8069.6000000000013</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44814</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J12" s="2">
@@ -984,7 +983,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E13" s="2">
@@ -992,19 +991,19 @@
         <v>8008.0000000000009</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44815</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J13" s="2">
@@ -1029,7 +1028,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E14" s="2">
@@ -1037,19 +1036,19 @@
         <v>7946.4000000000015</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44816</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J14" s="2">
@@ -1074,7 +1073,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E15" s="2">
@@ -1082,19 +1081,19 @@
         <v>7884.8000000000011</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J15" s="2">
@@ -1119,7 +1118,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E16" s="2">
@@ -1127,19 +1126,19 @@
         <v>7823.2000000000007</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44818</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J16" s="2">
@@ -1164,7 +1163,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E17" s="2">
@@ -1172,19 +1171,19 @@
         <v>7761.6000000000013</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44819</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J17" s="2">
@@ -1209,7 +1208,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E18" s="2">
@@ -1217,19 +1216,19 @@
         <v>7700.0000000000009</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44820</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J18" s="2">
@@ -1254,7 +1253,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E19" s="2">
@@ -1262,19 +1261,19 @@
         <v>7638.4000000000015</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44821</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J19" s="2">
@@ -1299,7 +1298,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E20" s="2">
@@ -1307,19 +1306,19 @@
         <v>7576.8000000000011</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44822</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J20" s="2">
@@ -1344,7 +1343,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E21" s="2">
@@ -1352,19 +1351,19 @@
         <v>7515.2000000000007</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44823</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J21" s="2">
@@ -1389,7 +1388,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E22" s="2">
@@ -1397,19 +1396,19 @@
         <v>7453.6000000000013</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44824</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J22" s="2">
@@ -1434,7 +1433,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E23" s="2">
@@ -1442,19 +1441,19 @@
         <v>7392.0000000000009</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44825</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J23" s="2">
@@ -1479,7 +1478,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E24" s="2">
@@ -1487,19 +1486,19 @@
         <v>7330.4000000000015</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44826</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J24" s="2">
@@ -1524,7 +1523,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E25" s="2">
@@ -1532,19 +1531,19 @@
         <v>7268.8000000000011</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44827</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J25" s="2">
@@ -1569,7 +1568,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E26" s="2">
@@ -1577,19 +1576,19 @@
         <v>7207.2000000000007</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44828</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J26" s="2">
@@ -1614,7 +1613,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E27" s="2">
@@ -1622,19 +1621,19 @@
         <v>7145.6000000000013</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44829</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J27" s="2">
@@ -1659,7 +1658,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E28" s="2">
@@ -1667,19 +1666,19 @@
         <v>7084.0000000000009</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44830</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J28" s="2">
@@ -1704,7 +1703,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E29" s="2">
@@ -1712,19 +1711,19 @@
         <v>7022.4000000000005</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44831</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J29" s="2">
@@ -1749,7 +1748,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E30" s="2">
@@ -1757,19 +1756,19 @@
         <v>6960.8000000000011</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44832</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J30" s="2">
@@ -1794,7 +1793,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E31" s="2">
@@ -1802,19 +1801,19 @@
         <v>6899.2000000000007</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44833</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J31" s="2">
@@ -1839,7 +1838,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E32" s="2">
@@ -1847,19 +1846,19 @@
         <v>6837.6000000000013</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44834</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J32" s="2">
@@ -1884,7 +1883,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E33" s="2">
@@ -1892,19 +1891,19 @@
         <v>6776.0000000000009</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44835</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J33" s="2">
@@ -1929,7 +1928,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E34" s="2">
@@ -1937,19 +1936,19 @@
         <v>6714.4000000000005</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44836</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J34" s="2">
@@ -1974,7 +1973,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E35" s="2">
@@ -1982,19 +1981,19 @@
         <v>3326.4000000000005</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44837</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J35" s="2">
@@ -2019,7 +2018,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E36" s="2">
@@ -2027,19 +2026,19 @@
         <v>3295.6000000000004</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44838</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J36" s="2">
@@ -2064,7 +2063,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E37" s="2">
@@ -2072,19 +2071,19 @@
         <v>3264.8000000000006</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44839</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J37" s="2">
@@ -2109,7 +2108,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E38" s="2">
@@ -2117,19 +2116,19 @@
         <v>3234.0000000000005</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>44840</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J38" s="2">

</xml_diff>

<commit_message>
Update 14. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0391CD-B0C5-4A56-8834-4F7E5AB7A604}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869E22BE-63B0-4C53-946C-FE66F3A9F1AB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,7 +172,7 @@
     <t>Фамилия квартиросъёмщика</t>
   </si>
   <si>
-    <t>Максимальная сумма, руб.</t>
+    <t>Максимальная сумма , руб.</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update 15. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869E22BE-63B0-4C53-946C-FE66F3A9F1AB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD21173-DF16-4C6C-B676-BFB4D2CEF532}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,7 +172,7 @@
     <t>Фамилия квартиросъёмщика</t>
   </si>
   <si>
-    <t>Максимальная сумма , руб.</t>
+    <t>Максимальная сумма, руб.</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="2">
-        <f>IF(A4&lt;33, D$3,D$3*0.5)</f>
+        <f>IF(A4&lt;33, D3,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="2">
@@ -623,7 +623,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D38" si="6">IF(A5&lt;33, D$3,D$3*0.5)</f>
+        <f t="shared" ref="D5:D38" si="6">IF(A5&lt;33, D4,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="2">

</xml_diff>

<commit_message>
Update 16. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD21173-DF16-4C6C-B676-BFB4D2CEF532}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA0564A-1F6F-481A-9AE9-6AFB06E9E798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="H4" sqref="H4:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="2">
-        <f>1.1*A1</f>
+        <f>112*1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="2">
@@ -578,7 +578,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="2">
-        <f>IF(A4&lt;33, D3,D$3*0.5)</f>
+        <f>IF(A3+1&lt;33, D3,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="2">
@@ -594,7 +594,7 @@
         <v>44806</v>
       </c>
       <c r="H4" s="2">
-        <f>IF(G4&lt;=F4, H3, H3+1)</f>
+        <f>IF(G3+1&lt;F3+1, H3, H3+1)</f>
         <v>0</v>
       </c>
       <c r="I4" s="2">
@@ -623,7 +623,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D38" si="6">IF(A5&lt;33, D4,D$3*0.5)</f>
+        <f t="shared" ref="D5:D38" si="6">IF(A4+1&lt;33, D4,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="2">
@@ -639,7 +639,7 @@
         <v>44807</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H38" si="9">IF(G5&lt;=F5, H4, H4+1)</f>
+        <f t="shared" ref="H5:H38" si="9">IF(G4+1&lt;F4+1, H4, H4+1)</f>
         <v>0</v>
       </c>
       <c r="I5" s="2">

</xml_diff>

<commit_message>
Update 17. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA0564A-1F6F-481A-9AE9-6AFB06E9E798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C04970-F8F9-409C-AF7A-82FA75DA7BE8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,9 +157,6 @@
     <t>Куропаткин 1</t>
   </si>
   <si>
-    <t>Куропаткин 2</t>
-  </si>
-  <si>
     <t>Общая сумма, руб.</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>Максимальная сумма, руб.</t>
+  </si>
+  <si>
+    <t>Кузин</t>
   </si>
 </sst>
 </file>
@@ -227,13 +227,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -457,13 +455,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
@@ -477,26 +475,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5">
+      <c r="A1" s="4">
         <v>112</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -530,37 +528,37 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
         <v>70</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <f>112*1.1</f>
         <v>123.20000000000002</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <f t="shared" ref="E3:E38" si="0">C3*D3</f>
         <v>8624.0000000000018</v>
       </c>
-      <c r="F3" s="3">
-        <v>44813</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="5">
+        <v>44813</v>
+      </c>
+      <c r="G3" s="5">
         <v>44805</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="2">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="4">
+        <v>10</v>
+      </c>
+      <c r="J3" s="4">
         <f t="shared" ref="J3:J38" si="1">H3*I3</f>
         <v>0</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="4">
         <f t="shared" ref="K3:K38" si="2">E3+J3</f>
         <v>8624.0000000000018</v>
       </c>
@@ -570,42 +568,42 @@
         <f t="shared" ref="A4:A38" si="3">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:C38" si="4">C3-0.5</f>
         <v>69.5</v>
       </c>
-      <c r="D4" s="2">
-        <f>IF(A3+1&lt;33, D3,D$3*0.5)</f>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="4">
+        <f>IF(A4&lt;33, D$3,D$3*0.5)</f>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>8562.4000000000015</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <f>F3</f>
         <v>44813</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <f>G3+1</f>
         <v>44806</v>
       </c>
-      <c r="H4" s="2">
-        <f>IF(G3+1&lt;F3+1, H3, H3+1)</f>
+      <c r="H4" s="4">
+        <f>IF(G4&lt;=F4, H3, H3+1)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <f t="shared" ref="I4:I38" si="5">I3</f>
         <v>10</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <f t="shared" si="2"/>
         <v>8562.4000000000015</v>
       </c>
@@ -615,42 +613,42 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <f t="shared" si="4"/>
         <v>69</v>
       </c>
-      <c r="D5" s="2">
-        <f t="shared" ref="D5:D38" si="6">IF(A4+1&lt;33, D4,D$3*0.5)</f>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="4">
+        <f t="shared" ref="D5:D38" si="6">IF(A5&lt;33, D$3,D$3*0.5)</f>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E5" s="4">
         <f t="shared" si="0"/>
         <v>8500.8000000000011</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <f t="shared" ref="F5:F38" si="7">F4</f>
         <v>44813</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="5">
         <f t="shared" ref="G5:G38" si="8">G4+1</f>
         <v>44807</v>
       </c>
-      <c r="H5" s="2">
-        <f t="shared" ref="H5:H38" si="9">IF(G4+1&lt;F4+1, H4, H4+1)</f>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5:H38" si="9">IF(G5&lt;=F5, H4, H4+1)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="I5" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J5" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <f t="shared" si="2"/>
         <v>8500.8000000000011</v>
       </c>
@@ -660,42 +658,42 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <f t="shared" si="4"/>
         <v>68.5</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E6" s="4">
         <f t="shared" si="0"/>
         <v>8439.2000000000007</v>
       </c>
-      <c r="F6" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G6" s="5">
         <f t="shared" si="8"/>
         <v>44808</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I6" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="I6" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J6" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="4">
         <f t="shared" si="2"/>
         <v>8439.2000000000007</v>
       </c>
@@ -705,42 +703,42 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="D7" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E7" s="4">
         <f t="shared" si="0"/>
         <v>8377.6</v>
       </c>
-      <c r="F7" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G7" s="5">
         <f t="shared" si="8"/>
         <v>44809</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I7" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="I7" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J7" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <f t="shared" si="2"/>
         <v>8377.6</v>
       </c>
@@ -750,42 +748,42 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
-      <c r="D8" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>8316.0000000000018</v>
       </c>
-      <c r="F8" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G8" s="5">
         <f t="shared" si="8"/>
         <v>44810</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I8" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="I8" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J8" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="4">
         <f t="shared" si="2"/>
         <v>8316.0000000000018</v>
       </c>
@@ -795,42 +793,42 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <f t="shared" si="4"/>
         <v>67</v>
       </c>
-      <c r="D9" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>8254.4000000000015</v>
       </c>
-      <c r="F9" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G9" s="5">
         <f t="shared" si="8"/>
         <v>44811</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I9" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="I9" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J9" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="4">
         <f t="shared" si="2"/>
         <v>8254.4000000000015</v>
       </c>
@@ -840,42 +838,42 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <f t="shared" si="4"/>
         <v>66.5</v>
       </c>
-      <c r="D10" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>8192.8000000000011</v>
       </c>
-      <c r="F10" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G10" s="5">
         <f t="shared" si="8"/>
         <v>44812</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I10" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="I10" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J10" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="4">
         <f t="shared" si="2"/>
         <v>8192.8000000000011</v>
       </c>
@@ -885,42 +883,42 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <f t="shared" si="4"/>
         <v>66</v>
       </c>
-      <c r="D11" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="D11" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E11" s="4">
         <f t="shared" si="0"/>
         <v>8131.2000000000007</v>
       </c>
-      <c r="F11" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G11" s="3">
-        <f t="shared" si="8"/>
-        <v>44813</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="F11" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="8"/>
+        <v>44813</v>
+      </c>
+      <c r="H11" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I11" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="I11" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J11" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="4">
         <f t="shared" si="2"/>
         <v>8131.2000000000007</v>
       </c>
@@ -930,42 +928,42 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <f t="shared" si="4"/>
         <v>65.5</v>
       </c>
-      <c r="D12" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E12" s="4">
         <f t="shared" si="0"/>
         <v>8069.6000000000013</v>
       </c>
-      <c r="F12" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="8"/>
         <v>44814</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="4">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="I12" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J12" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="K12" s="2">
+      <c r="I12" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K12" s="4">
         <f t="shared" si="2"/>
         <v>8079.6000000000013</v>
       </c>
@@ -975,42 +973,42 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="D13" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>8008.0000000000009</v>
       </c>
-      <c r="F13" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F13" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G13" s="5">
         <f t="shared" si="8"/>
         <v>44815</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="4">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="I13" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="I13" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J13" s="4">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="4">
         <f t="shared" si="2"/>
         <v>8028.0000000000009</v>
       </c>
@@ -1020,42 +1018,42 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <f t="shared" si="4"/>
         <v>64.5</v>
       </c>
-      <c r="D14" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E14" s="4">
         <f t="shared" si="0"/>
         <v>7946.4000000000015</v>
       </c>
-      <c r="F14" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F14" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" si="8"/>
         <v>44816</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="4">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="I14" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="I14" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="4">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="4">
         <f t="shared" si="2"/>
         <v>7976.4000000000015</v>
       </c>
@@ -1065,42 +1063,42 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-      <c r="D15" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="D15" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E15" s="4">
         <f t="shared" si="0"/>
         <v>7884.8000000000011</v>
       </c>
-      <c r="F15" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="F15" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="8"/>
         <v>44817</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="4">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="I15" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="I15" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J15" s="4">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="4">
         <f t="shared" si="2"/>
         <v>7924.8000000000011</v>
       </c>
@@ -1110,42 +1108,42 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" si="4"/>
         <v>63.5</v>
       </c>
-      <c r="D16" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E16" s="4">
         <f t="shared" si="0"/>
         <v>7823.2000000000007</v>
       </c>
-      <c r="F16" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F16" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G16" s="5">
         <f t="shared" si="8"/>
         <v>44818</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="4">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="I16" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="I16" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J16" s="4">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="4">
         <f t="shared" si="2"/>
         <v>7873.2000000000007</v>
       </c>
@@ -1155,42 +1153,42 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <f t="shared" si="4"/>
         <v>63</v>
       </c>
-      <c r="D17" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="D17" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E17" s="4">
         <f t="shared" si="0"/>
         <v>7761.6000000000013</v>
       </c>
-      <c r="F17" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="F17" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G17" s="5">
         <f t="shared" si="8"/>
         <v>44819</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="4">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="I17" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="I17" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J17" s="4">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="4">
         <f t="shared" si="2"/>
         <v>7821.6000000000013</v>
       </c>
@@ -1200,42 +1198,42 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="4">
         <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
-      <c r="D18" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="D18" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E18" s="4">
         <f t="shared" si="0"/>
         <v>7700.0000000000009</v>
       </c>
-      <c r="F18" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="F18" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G18" s="5">
         <f t="shared" si="8"/>
         <v>44820</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="4">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="I18" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="I18" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J18" s="4">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="4">
         <f t="shared" si="2"/>
         <v>7770.0000000000009</v>
       </c>
@@ -1245,42 +1243,42 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <f t="shared" si="4"/>
         <v>62</v>
       </c>
-      <c r="D19" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D19" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E19" s="4">
         <f t="shared" si="0"/>
         <v>7638.4000000000015</v>
       </c>
-      <c r="F19" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F19" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G19" s="5">
         <f t="shared" si="8"/>
         <v>44821</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="4">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="I19" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="I19" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J19" s="4">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="4">
         <f t="shared" si="2"/>
         <v>7718.4000000000015</v>
       </c>
@@ -1290,42 +1288,42 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="4">
         <f t="shared" si="4"/>
         <v>61.5</v>
       </c>
-      <c r="D20" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D20" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E20" s="4">
         <f t="shared" si="0"/>
         <v>7576.8000000000011</v>
       </c>
-      <c r="F20" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="F20" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G20" s="5">
         <f t="shared" si="8"/>
         <v>44822</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="4">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="I20" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J20" s="2">
+      <c r="I20" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J20" s="4">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="4">
         <f t="shared" si="2"/>
         <v>7666.8000000000011</v>
       </c>
@@ -1335,42 +1333,42 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="4">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="D21" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="D21" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E21" s="4">
         <f t="shared" si="0"/>
         <v>7515.2000000000007</v>
       </c>
-      <c r="F21" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="F21" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G21" s="5">
         <f t="shared" si="8"/>
         <v>44823</v>
       </c>
-      <c r="H21" s="2">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="I21" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J21" s="2">
+      <c r="H21" s="4">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J21" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="4">
         <f t="shared" si="2"/>
         <v>7615.2000000000007</v>
       </c>
@@ -1380,42 +1378,42 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <f t="shared" si="4"/>
         <v>60.5</v>
       </c>
-      <c r="D22" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="D22" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E22" s="4">
         <f t="shared" si="0"/>
         <v>7453.6000000000013</v>
       </c>
-      <c r="F22" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G22" s="5">
         <f t="shared" si="8"/>
         <v>44824</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="4">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
-      <c r="I22" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J22" s="2">
+      <c r="I22" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J22" s="4">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="4">
         <f t="shared" si="2"/>
         <v>7563.6000000000013</v>
       </c>
@@ -1425,42 +1423,42 @@
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="D23" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D23" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E23" s="4">
         <f t="shared" si="0"/>
         <v>7392.0000000000009</v>
       </c>
-      <c r="F23" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G23" s="3">
+      <c r="F23" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G23" s="5">
         <f t="shared" si="8"/>
         <v>44825</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="4">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="I23" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J23" s="2">
+      <c r="I23" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J23" s="4">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="4">
         <f t="shared" si="2"/>
         <v>7512.0000000000009</v>
       </c>
@@ -1470,42 +1468,42 @@
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="4">
         <f t="shared" si="4"/>
         <v>59.5</v>
       </c>
-      <c r="D24" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E24" s="4">
         <f t="shared" si="0"/>
         <v>7330.4000000000015</v>
       </c>
-      <c r="F24" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="F24" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G24" s="5">
         <f t="shared" si="8"/>
         <v>44826</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="4">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="I24" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J24" s="2">
+      <c r="I24" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J24" s="4">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="4">
         <f t="shared" si="2"/>
         <v>7460.4000000000015</v>
       </c>
@@ -1515,42 +1513,42 @@
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="4">
         <f t="shared" si="4"/>
         <v>59</v>
       </c>
-      <c r="D25" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E25" s="4">
         <f t="shared" si="0"/>
         <v>7268.8000000000011</v>
       </c>
-      <c r="F25" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G25" s="3">
+      <c r="F25" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G25" s="5">
         <f t="shared" si="8"/>
         <v>44827</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="4">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="I25" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J25" s="2">
+      <c r="I25" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J25" s="4">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="4">
         <f t="shared" si="2"/>
         <v>7408.8000000000011</v>
       </c>
@@ -1560,42 +1558,42 @@
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="4">
         <f t="shared" si="4"/>
         <v>58.5</v>
       </c>
-      <c r="D26" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="D26" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E26" s="4">
         <f t="shared" si="0"/>
         <v>7207.2000000000007</v>
       </c>
-      <c r="F26" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G26" s="3">
+      <c r="F26" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G26" s="5">
         <f t="shared" si="8"/>
         <v>44828</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="4">
         <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="I26" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J26" s="2">
+      <c r="I26" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J26" s="4">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="4">
         <f t="shared" si="2"/>
         <v>7357.2000000000007</v>
       </c>
@@ -1605,42 +1603,42 @@
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="4">
         <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="D27" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E27" s="2">
+      <c r="D27" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E27" s="4">
         <f t="shared" si="0"/>
         <v>7145.6000000000013</v>
       </c>
-      <c r="F27" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G27" s="3">
+      <c r="F27" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G27" s="5">
         <f t="shared" si="8"/>
         <v>44829</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="4">
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="I27" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J27" s="2">
+      <c r="I27" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J27" s="4">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="4">
         <f t="shared" si="2"/>
         <v>7305.6000000000013</v>
       </c>
@@ -1650,42 +1648,42 @@
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="4">
         <f t="shared" si="4"/>
         <v>57.5</v>
       </c>
-      <c r="D28" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="D28" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E28" s="4">
         <f t="shared" si="0"/>
         <v>7084.0000000000009</v>
       </c>
-      <c r="F28" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G28" s="3">
+      <c r="F28" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G28" s="5">
         <f t="shared" si="8"/>
         <v>44830</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="4">
         <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="I28" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J28" s="2">
+      <c r="I28" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J28" s="4">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="4">
         <f t="shared" si="2"/>
         <v>7254.0000000000009</v>
       </c>
@@ -1695,42 +1693,42 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="4">
         <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="D29" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="D29" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E29" s="4">
         <f t="shared" si="0"/>
         <v>7022.4000000000005</v>
       </c>
-      <c r="F29" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G29" s="3">
+      <c r="F29" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G29" s="5">
         <f t="shared" si="8"/>
         <v>44831</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="4">
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="I29" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J29" s="2">
+      <c r="I29" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J29" s="4">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="4">
         <f t="shared" si="2"/>
         <v>7202.4000000000005</v>
       </c>
@@ -1740,42 +1738,42 @@
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="4">
         <f t="shared" si="4"/>
         <v>56.5</v>
       </c>
-      <c r="D30" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="D30" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E30" s="4">
         <f t="shared" si="0"/>
         <v>6960.8000000000011</v>
       </c>
-      <c r="F30" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G30" s="3">
+      <c r="F30" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G30" s="5">
         <f t="shared" si="8"/>
         <v>44832</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="4">
         <f t="shared" si="9"/>
         <v>19</v>
       </c>
-      <c r="I30" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J30" s="2">
+      <c r="I30" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J30" s="4">
         <f t="shared" si="1"/>
         <v>190</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="4">
         <f t="shared" si="2"/>
         <v>7150.8000000000011</v>
       </c>
@@ -1785,42 +1783,42 @@
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="4">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="D31" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E31" s="2">
+      <c r="D31" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E31" s="4">
         <f t="shared" si="0"/>
         <v>6899.2000000000007</v>
       </c>
-      <c r="F31" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="F31" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G31" s="5">
         <f t="shared" si="8"/>
         <v>44833</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="4">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
-      <c r="I31" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J31" s="2">
+      <c r="I31" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J31" s="4">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="4">
         <f t="shared" si="2"/>
         <v>7099.2000000000007</v>
       </c>
@@ -1830,42 +1828,42 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="4">
         <f t="shared" si="4"/>
         <v>55.5</v>
       </c>
-      <c r="D32" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="D32" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E32" s="4">
         <f t="shared" si="0"/>
         <v>6837.6000000000013</v>
       </c>
-      <c r="F32" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="F32" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G32" s="5">
         <f t="shared" si="8"/>
         <v>44834</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="4">
         <f t="shared" si="9"/>
         <v>21</v>
       </c>
-      <c r="I32" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J32" s="2">
+      <c r="I32" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J32" s="4">
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="4">
         <f t="shared" si="2"/>
         <v>7047.6000000000013</v>
       </c>
@@ -1875,42 +1873,42 @@
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="4">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="D33" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="D33" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E33" s="4">
         <f t="shared" si="0"/>
         <v>6776.0000000000009</v>
       </c>
-      <c r="F33" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G33" s="3">
+      <c r="F33" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G33" s="5">
         <f t="shared" si="8"/>
         <v>44835</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="4">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="I33" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J33" s="2">
+      <c r="I33" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J33" s="4">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="4">
         <f t="shared" si="2"/>
         <v>6996.0000000000009</v>
       </c>
@@ -1920,42 +1918,42 @@
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="4">
         <f t="shared" si="4"/>
         <v>54.5</v>
       </c>
-      <c r="D34" s="2">
-        <f t="shared" si="6"/>
-        <v>123.20000000000002</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="D34" s="4">
+        <f t="shared" si="6"/>
+        <v>123.20000000000002</v>
+      </c>
+      <c r="E34" s="4">
         <f t="shared" si="0"/>
         <v>6714.4000000000005</v>
       </c>
-      <c r="F34" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G34" s="3">
+      <c r="F34" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G34" s="5">
         <f t="shared" si="8"/>
         <v>44836</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="4">
         <f t="shared" si="9"/>
         <v>23</v>
       </c>
-      <c r="I34" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J34" s="2">
+      <c r="I34" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J34" s="4">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="4">
         <f t="shared" si="2"/>
         <v>6944.4000000000005</v>
       </c>
@@ -1965,42 +1963,42 @@
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="4">
         <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="4">
         <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="4">
         <f t="shared" si="0"/>
         <v>3326.4000000000005</v>
       </c>
-      <c r="F35" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G35" s="3">
+      <c r="F35" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G35" s="5">
         <f t="shared" si="8"/>
         <v>44837</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="4">
         <f t="shared" si="9"/>
         <v>24</v>
       </c>
-      <c r="I35" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J35" s="2">
+      <c r="I35" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J35" s="4">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="4">
         <f t="shared" si="2"/>
         <v>3566.4000000000005</v>
       </c>
@@ -2010,42 +2008,42 @@
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="4">
         <f t="shared" si="4"/>
         <v>53.5</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="4">
         <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="4">
         <f t="shared" si="0"/>
         <v>3295.6000000000004</v>
       </c>
-      <c r="F36" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G36" s="3">
+      <c r="F36" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G36" s="5">
         <f t="shared" si="8"/>
         <v>44838</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="4">
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="I36" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J36" s="2">
+      <c r="I36" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J36" s="4">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="4">
         <f t="shared" si="2"/>
         <v>3545.6000000000004</v>
       </c>
@@ -2055,42 +2053,42 @@
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="B37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="4">
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="4">
         <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="4">
         <f t="shared" si="0"/>
         <v>3264.8000000000006</v>
       </c>
-      <c r="F37" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G37" s="3">
+      <c r="F37" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G37" s="5">
         <f t="shared" si="8"/>
         <v>44839</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="4">
         <f t="shared" si="9"/>
         <v>26</v>
       </c>
-      <c r="I37" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J37" s="2">
+      <c r="I37" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J37" s="4">
         <f t="shared" si="1"/>
         <v>260</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="4">
         <f t="shared" si="2"/>
         <v>3524.8000000000006</v>
       </c>
@@ -2100,130 +2098,130 @@
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="4"/>
+        <v>52.5</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="6"/>
+        <v>61.600000000000009</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="0"/>
+        <v>3234.0000000000005</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G38" s="5">
+        <f t="shared" si="8"/>
+        <v>44840</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="I38" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="K38" s="4">
+        <f t="shared" si="2"/>
+        <v>3504.0000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="2">
-        <f t="shared" si="4"/>
-        <v>52.5</v>
-      </c>
-      <c r="D38" s="2">
-        <f t="shared" si="6"/>
-        <v>61.600000000000009</v>
-      </c>
-      <c r="E38" s="2">
-        <f t="shared" si="0"/>
-        <v>3234.0000000000005</v>
-      </c>
-      <c r="F38" s="3">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G38" s="3">
-        <f t="shared" si="8"/>
-        <v>44840</v>
-      </c>
-      <c r="H38" s="2">
-        <f t="shared" si="9"/>
-        <v>27</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="J38" s="2">
-        <f t="shared" si="1"/>
-        <v>270</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="2"/>
-        <v>3504.0000000000005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2">
+        <f>TRUNC(SUM(K3:K38))</f>
+        <v>262315</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C40" s="2">
-        <f>INT(SUM(K3:K38))</f>
-        <v>262315</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C41" s="2">
         <f>AVERAGE(C3:C38)</f>
         <v>61.25</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="2">
         <f>MAX(H3:H38)</f>
         <v>27</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
+      <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="2">
         <f>MAX(K3:K38)</f>
         <v>8624.0000000000018</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.70000004768371604" right="0.70000004768371604" top="0.75" bottom="0.75" header="0.30000001192092901" footer="0.30000001192092901"/>

</xml_diff>

<commit_message>
Update 18. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C04970-F8F9-409C-AF7A-82FA75DA7BE8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A061A32-74C9-43F8-AA6B-00CDE0621E78}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,7 +2211,7 @@
         <v>49</v>
       </c>
       <c r="C43" s="2">
-        <f>MAX(K3:K38)</f>
+        <f>MAX(E3:E38)</f>
         <v>8624.0000000000018</v>
       </c>
       <c r="D43" s="3"/>

</xml_diff>

<commit_message>
Update 19. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A061A32-74C9-43F8-AA6B-00CDE0621E78}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC5FB2D-201C-4CDB-9274-4AFAE7E241B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>112*1.1</f>
+        <f>IF(A3&lt;33,A$1*1.1,A$1*0.55)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -576,7 +576,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f>IF(A4&lt;33, D$3,D$3*0.5)</f>
+        <f t="shared" ref="D4:D38" si="5">IF(A4&lt;33,A$1*1.1,A$1*0.55)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I38" si="5">I3</f>
+        <f t="shared" ref="I4:I38" si="6">I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="4">
@@ -621,7 +621,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D38" si="6">IF(A5&lt;33, D$3,D$3*0.5)</f>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="4">
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J5" s="4">
@@ -666,7 +666,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E6" s="4">
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J6" s="4">
@@ -711,7 +711,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E7" s="4">
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J7" s="4">
@@ -756,7 +756,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E8" s="4">
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J8" s="4">
@@ -801,7 +801,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E9" s="4">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J9" s="4">
@@ -846,7 +846,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E10" s="4">
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J10" s="4">
@@ -891,7 +891,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E11" s="4">
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J11" s="4">
@@ -936,7 +936,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E12" s="4">
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J12" s="4">
@@ -981,7 +981,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E13" s="4">
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J13" s="4">
@@ -1026,7 +1026,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E14" s="4">
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J14" s="4">
@@ -1071,7 +1071,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E15" s="4">
@@ -1091,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J15" s="4">
@@ -1116,7 +1116,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E16" s="4">
@@ -1136,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J16" s="4">
@@ -1161,7 +1161,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E17" s="4">
@@ -1181,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J17" s="4">
@@ -1206,7 +1206,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E18" s="4">
@@ -1226,7 +1226,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J18" s="4">
@@ -1251,7 +1251,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E19" s="4">
@@ -1271,7 +1271,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J19" s="4">
@@ -1296,7 +1296,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E20" s="4">
@@ -1316,7 +1316,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J20" s="4">
@@ -1341,7 +1341,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E21" s="4">
@@ -1361,7 +1361,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J21" s="4">
@@ -1386,7 +1386,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E22" s="4">
@@ -1406,7 +1406,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J22" s="4">
@@ -1431,7 +1431,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E23" s="4">
@@ -1451,7 +1451,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J23" s="4">
@@ -1476,7 +1476,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E24" s="4">
@@ -1496,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J24" s="4">
@@ -1521,7 +1521,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E25" s="4">
@@ -1541,7 +1541,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J25" s="4">
@@ -1566,7 +1566,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E26" s="4">
@@ -1586,7 +1586,7 @@
         <v>15</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J26" s="4">
@@ -1611,7 +1611,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E27" s="4">
@@ -1631,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J27" s="4">
@@ -1656,7 +1656,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E28" s="4">
@@ -1676,7 +1676,7 @@
         <v>17</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J28" s="4">
@@ -1701,7 +1701,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E29" s="4">
@@ -1721,7 +1721,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J29" s="4">
@@ -1746,7 +1746,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E30" s="4">
@@ -1766,7 +1766,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J30" s="4">
@@ -1791,7 +1791,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E31" s="4">
@@ -1811,7 +1811,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J31" s="4">
@@ -1836,7 +1836,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E32" s="4">
@@ -1856,7 +1856,7 @@
         <v>21</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J32" s="4">
@@ -1881,7 +1881,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E33" s="4">
@@ -1901,7 +1901,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J33" s="4">
@@ -1926,7 +1926,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E34" s="4">
@@ -1946,7 +1946,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J34" s="4">
@@ -1971,7 +1971,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E35" s="4">
@@ -1991,7 +1991,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J35" s="4">
@@ -2016,7 +2016,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E36" s="4">
@@ -2036,7 +2036,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J36" s="4">
@@ -2061,7 +2061,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E37" s="4">
@@ -2081,7 +2081,7 @@
         <v>26</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J37" s="4">
@@ -2106,7 +2106,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E38" s="4">
@@ -2126,7 +2126,7 @@
         <v>27</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J38" s="4">
@@ -2211,7 +2211,7 @@
         <v>49</v>
       </c>
       <c r="C43" s="2">
-        <f>MAX(E3:E38)</f>
+        <f>MAX(K3:K38)</f>
         <v>8624.0000000000018</v>
       </c>
       <c r="D43" s="3"/>

</xml_diff>

<commit_message>
Update 20. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC5FB2D-201C-4CDB-9274-4AFAE7E241B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369813AC-9204-490D-8369-81716745D730}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>IF(A3&lt;33,A$1*1.1,A$1*0.55)</f>
+        <f>IF(A3&lt;33,A$1*1.1,A$1*1.1/2)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -576,7 +576,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D38" si="5">IF(A4&lt;33,A$1*1.1,A$1*0.55)</f>
+        <f t="shared" ref="D4:D38" si="5">IF(A4&lt;33,A$1*1.1,A$1*1.1/2)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">

</xml_diff>

<commit_message>
Update 21. table_1_112.xlsx edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369813AC-9204-490D-8369-81716745D730}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD91F91-F8BD-4A3E-8A87-F4228DB6D798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>IF(A3&lt;33,A$1*1.1,A$1*1.1/2)</f>
+        <f>A1*1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -576,7 +576,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D38" si="5">IF(A4&lt;33,A$1*1.1,A$1*1.1/2)</f>
+        <f>IF(A3+1&lt;33,D$3,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">
@@ -592,11 +592,11 @@
         <v>44806</v>
       </c>
       <c r="H4" s="4">
-        <f>IF(G4&lt;=F4, H3, H3+1)</f>
+        <f>IF(G3+1&lt;F3+1, H3, H3+1)</f>
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I38" si="6">I3</f>
+        <f t="shared" ref="I4:I38" si="5">I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="4">
@@ -621,7 +621,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D5:D38" si="6">IF(A4+1&lt;33,D$3,D$3*0.5)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="4">
@@ -637,11 +637,11 @@
         <v>44807</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ref="H5:H38" si="9">IF(G5&lt;=F5, H4, H4+1)</f>
+        <f t="shared" ref="H5:H38" si="9">IF(G4+1&lt;F4+1, H4, H4+1)</f>
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J5" s="4">
@@ -666,7 +666,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E6" s="4">
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J6" s="4">
@@ -711,7 +711,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E7" s="4">
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J7" s="4">
@@ -756,7 +756,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E8" s="4">
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J8" s="4">
@@ -801,7 +801,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E9" s="4">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J9" s="4">
@@ -846,7 +846,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E10" s="4">
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J10" s="4">
@@ -891,7 +891,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E11" s="4">
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J11" s="4">
@@ -936,7 +936,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E12" s="4">
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J12" s="4">
@@ -981,7 +981,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E13" s="4">
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J13" s="4">
@@ -1026,7 +1026,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E14" s="4">
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J14" s="4">
@@ -1071,7 +1071,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E15" s="4">
@@ -1091,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J15" s="4">
@@ -1116,7 +1116,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E16" s="4">
@@ -1136,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J16" s="4">
@@ -1161,7 +1161,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E17" s="4">
@@ -1181,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J17" s="4">
@@ -1206,7 +1206,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E18" s="4">
@@ -1226,7 +1226,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J18" s="4">
@@ -1251,7 +1251,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E19" s="4">
@@ -1271,7 +1271,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J19" s="4">
@@ -1296,7 +1296,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E20" s="4">
@@ -1316,7 +1316,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J20" s="4">
@@ -1341,7 +1341,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E21" s="4">
@@ -1361,7 +1361,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J21" s="4">
@@ -1386,7 +1386,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E22" s="4">
@@ -1406,7 +1406,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J22" s="4">
@@ -1431,7 +1431,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E23" s="4">
@@ -1451,7 +1451,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J23" s="4">
@@ -1476,7 +1476,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E24" s="4">
@@ -1496,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J24" s="4">
@@ -1521,7 +1521,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E25" s="4">
@@ -1541,7 +1541,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J25" s="4">
@@ -1566,7 +1566,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E26" s="4">
@@ -1586,7 +1586,7 @@
         <v>15</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J26" s="4">
@@ -1611,7 +1611,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E27" s="4">
@@ -1631,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J27" s="4">
@@ -1656,7 +1656,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E28" s="4">
@@ -1676,7 +1676,7 @@
         <v>17</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J28" s="4">
@@ -1701,7 +1701,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E29" s="4">
@@ -1721,7 +1721,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J29" s="4">
@@ -1746,7 +1746,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E30" s="4">
@@ -1766,7 +1766,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J30" s="4">
@@ -1791,7 +1791,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E31" s="4">
@@ -1811,7 +1811,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J31" s="4">
@@ -1836,7 +1836,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E32" s="4">
@@ -1856,7 +1856,7 @@
         <v>21</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J32" s="4">
@@ -1881,7 +1881,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E33" s="4">
@@ -1901,7 +1901,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J33" s="4">
@@ -1926,7 +1926,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E34" s="4">
@@ -1946,7 +1946,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J34" s="4">
@@ -1971,7 +1971,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E35" s="4">
@@ -1991,7 +1991,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J35" s="4">
@@ -2016,7 +2016,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E36" s="4">
@@ -2036,7 +2036,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J36" s="4">
@@ -2061,7 +2061,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E37" s="4">
@@ -2081,7 +2081,7 @@
         <v>26</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J37" s="4">
@@ -2106,7 +2106,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E38" s="4">
@@ -2126,7 +2126,7 @@
         <v>27</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J38" s="4">

</xml_diff>

<commit_message>
Update 21. edited table 1
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20390"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD91F91-F8BD-4A3E-8A87-F4228DB6D798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A021D68A-4CAF-4537-9B99-385F8E6D4246}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,6 +549,7 @@
         <v>44805</v>
       </c>
       <c r="H3" s="4">
+        <f>0</f>
         <v>0</v>
       </c>
       <c r="I3" s="4">

</xml_diff>

<commit_message>
Update 22. edited table 1
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A021D68A-4CAF-4537-9B99-385F8E6D4246}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4669382-7A20-452B-88BB-EC5B4406044B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>A1*1.1</f>
+        <f>A$1*1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -549,7 +549,7 @@
         <v>44805</v>
       </c>
       <c r="H3" s="4">
-        <f>0</f>
+        <f>A1*0</f>
         <v>0</v>
       </c>
       <c r="I3" s="4">
@@ -577,7 +577,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f>IF(A3+1&lt;33,D$3,D$3*0.5)</f>
+        <f t="shared" ref="D4:D34" si="5">A$1*1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">
@@ -593,11 +593,11 @@
         <v>44806</v>
       </c>
       <c r="H4" s="4">
-        <f>IF(G3+1&lt;F3+1, H3, H3+1)</f>
+        <f>IF(G4&lt;F4, H$3, G4-F4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I38" si="5">I3</f>
+        <f t="shared" ref="I4:I38" si="6">I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="4">
@@ -622,7 +622,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D38" si="6">IF(A4+1&lt;33,D$3,D$3*0.5)</f>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="4">
@@ -638,11 +638,11 @@
         <v>44807</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ref="H5:H38" si="9">IF(G4+1&lt;F4+1, H4, H4+1)</f>
+        <f t="shared" ref="H5:H38" si="9">IF(G5&lt;F5, H$3, G5-F5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J5" s="4">
@@ -667,7 +667,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E6" s="4">
@@ -687,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J6" s="4">
@@ -712,7 +712,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E7" s="4">
@@ -732,7 +732,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J7" s="4">
@@ -757,7 +757,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E8" s="4">
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J8" s="4">
@@ -802,7 +802,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E9" s="4">
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J9" s="4">
@@ -847,7 +847,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E10" s="4">
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J10" s="4">
@@ -892,7 +892,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E11" s="4">
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J11" s="4">
@@ -937,7 +937,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E12" s="4">
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J12" s="4">
@@ -982,7 +982,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E13" s="4">
@@ -1002,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J13" s="4">
@@ -1027,7 +1027,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E14" s="4">
@@ -1047,7 +1047,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J14" s="4">
@@ -1072,7 +1072,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E15" s="4">
@@ -1092,7 +1092,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J15" s="4">
@@ -1117,7 +1117,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E16" s="4">
@@ -1137,7 +1137,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J16" s="4">
@@ -1162,7 +1162,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E17" s="4">
@@ -1182,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J17" s="4">
@@ -1207,7 +1207,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E18" s="4">
@@ -1227,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J18" s="4">
@@ -1252,7 +1252,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E19" s="4">
@@ -1272,7 +1272,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J19" s="4">
@@ -1297,7 +1297,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E20" s="4">
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J20" s="4">
@@ -1342,7 +1342,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E21" s="4">
@@ -1362,7 +1362,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J21" s="4">
@@ -1387,7 +1387,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E22" s="4">
@@ -1407,7 +1407,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J22" s="4">
@@ -1432,7 +1432,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E23" s="4">
@@ -1452,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J23" s="4">
@@ -1477,7 +1477,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E24" s="4">
@@ -1497,7 +1497,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J24" s="4">
@@ -1522,7 +1522,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E25" s="4">
@@ -1542,7 +1542,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J25" s="4">
@@ -1567,7 +1567,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E26" s="4">
@@ -1587,7 +1587,7 @@
         <v>15</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J26" s="4">
@@ -1612,7 +1612,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E27" s="4">
@@ -1632,7 +1632,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J27" s="4">
@@ -1657,7 +1657,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E28" s="4">
@@ -1677,7 +1677,7 @@
         <v>17</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J28" s="4">
@@ -1702,7 +1702,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E29" s="4">
@@ -1722,7 +1722,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J29" s="4">
@@ -1747,7 +1747,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E30" s="4">
@@ -1767,7 +1767,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J30" s="4">
@@ -1792,7 +1792,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E31" s="4">
@@ -1812,7 +1812,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J31" s="4">
@@ -1837,7 +1837,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E32" s="4">
@@ -1857,7 +1857,7 @@
         <v>21</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J32" s="4">
@@ -1882,7 +1882,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E33" s="4">
@@ -1902,7 +1902,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J33" s="4">
@@ -1927,7 +1927,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E34" s="4">
@@ -1947,7 +1947,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J34" s="4">
@@ -1972,7 +1972,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="6"/>
+        <f>A$1*0.55</f>
         <v>61.600000000000009</v>
       </c>
       <c r="E35" s="4">
@@ -1992,7 +1992,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J35" s="4">
@@ -2017,7 +2017,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D36:D38" si="10">A$1*0.55</f>
         <v>61.600000000000009</v>
       </c>
       <c r="E36" s="4">
@@ -2037,7 +2037,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J36" s="4">
@@ -2062,7 +2062,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E37" s="4">
@@ -2082,7 +2082,7 @@
         <v>26</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J37" s="4">
@@ -2107,7 +2107,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E38" s="4">
@@ -2127,7 +2127,7 @@
         <v>27</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J38" s="4">

</xml_diff>

<commit_message>
Update 23. table1 edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4669382-7A20-452B-88BB-EC5B4406044B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7AA4A0-030E-4FAF-BE7D-5267A8D7DE01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>A$1*1.1</f>
+        <f>IF(A3 &lt; 33,A$1*1.1, A$1 * 0.55)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -549,7 +549,7 @@
         <v>44805</v>
       </c>
       <c r="H3" s="4">
-        <f>A1*0</f>
+        <f>0</f>
         <v>0</v>
       </c>
       <c r="I3" s="4">
@@ -577,7 +577,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D34" si="5">A$1*1.1</f>
+        <f t="shared" ref="D4:D38" si="5">IF(A4 &lt; 33,A$1*1.1, A$1 * 0.55)</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">
@@ -1972,7 +1972,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4">
-        <f>A$1*0.55</f>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E35" s="4">
@@ -2017,7 +2017,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" ref="D36:D38" si="10">A$1*0.55</f>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E36" s="4">
@@ -2062,7 +2062,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E37" s="4">
@@ -2107,7 +2107,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E38" s="4">

</xml_diff>

<commit_message>
Update 24. table1 edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7AA4A0-030E-4FAF-BE7D-5267A8D7DE01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB2C70-8989-48E4-9510-E6D3A0369862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>IF(A3 &lt; 33,A$1*1.1, A$1 * 0.55)</f>
+        <f>A$1 * 1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -549,7 +549,7 @@
         <v>44805</v>
       </c>
       <c r="H3" s="4">
-        <f>0</f>
+        <f>IF(G3&gt;F3,G3-F3,0)</f>
         <v>0</v>
       </c>
       <c r="I3" s="4">
@@ -577,7 +577,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D38" si="5">IF(A4 &lt; 33,A$1*1.1, A$1 * 0.55)</f>
+        <f t="shared" ref="D4:D34" si="5">A$1 * 1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">
@@ -593,11 +593,11 @@
         <v>44806</v>
       </c>
       <c r="H4" s="4">
-        <f>IF(G4&lt;F4, H$3, G4-F4)</f>
+        <f t="shared" ref="H4:H38" si="6">IF(G4&gt;F4,G4-F4,0)</f>
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I38" si="6">I3</f>
+        <f t="shared" ref="I4:I38" si="7">I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="4">
@@ -630,19 +630,19 @@
         <v>8500.8000000000011</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F38" si="7">F4</f>
+        <f t="shared" ref="F5:F38" si="8">F4</f>
         <v>44813</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G38" si="8">G4+1</f>
+        <f t="shared" ref="G5:G38" si="9">G4+1</f>
         <v>44807</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ref="H5:H38" si="9">IF(G5&lt;F5, H$3, G5-F5)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J5" s="4">
@@ -675,19 +675,19 @@
         <v>8439.2000000000007</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44808</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J6" s="4">
@@ -720,19 +720,19 @@
         <v>8377.6</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44809</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J7" s="4">
@@ -765,19 +765,19 @@
         <v>8316.0000000000018</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44810</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J8" s="4">
@@ -810,19 +810,19 @@
         <v>8254.4000000000015</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44811</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J9" s="4">
@@ -855,19 +855,19 @@
         <v>8192.8000000000011</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44812</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J10" s="4">
@@ -900,19 +900,19 @@
         <v>8131.2000000000007</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44813</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J11" s="4">
@@ -945,19 +945,19 @@
         <v>8069.6000000000013</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44814</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J12" s="4">
@@ -990,19 +990,19 @@
         <v>8008.0000000000009</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44815</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J13" s="4">
@@ -1035,19 +1035,19 @@
         <v>7946.4000000000015</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44816</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J14" s="4">
@@ -1080,19 +1080,19 @@
         <v>7884.8000000000011</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J15" s="4">
@@ -1125,19 +1125,19 @@
         <v>7823.2000000000007</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44818</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J16" s="4">
@@ -1170,19 +1170,19 @@
         <v>7761.6000000000013</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44819</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J17" s="4">
@@ -1215,19 +1215,19 @@
         <v>7700.0000000000009</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44820</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J18" s="4">
@@ -1260,19 +1260,19 @@
         <v>7638.4000000000015</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44821</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J19" s="4">
@@ -1305,19 +1305,19 @@
         <v>7576.8000000000011</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44822</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J20" s="4">
@@ -1350,19 +1350,19 @@
         <v>7515.2000000000007</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44823</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J21" s="4">
@@ -1395,19 +1395,19 @@
         <v>7453.6000000000013</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G22" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44824</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J22" s="4">
@@ -1440,19 +1440,19 @@
         <v>7392.0000000000009</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G23" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44825</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J23" s="4">
@@ -1485,19 +1485,19 @@
         <v>7330.4000000000015</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44826</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J24" s="4">
@@ -1530,19 +1530,19 @@
         <v>7268.8000000000011</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44827</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J25" s="4">
@@ -1575,19 +1575,19 @@
         <v>7207.2000000000007</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44828</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J26" s="4">
@@ -1620,19 +1620,19 @@
         <v>7145.6000000000013</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G27" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44829</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J27" s="4">
@@ -1665,19 +1665,19 @@
         <v>7084.0000000000009</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44830</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J28" s="4">
@@ -1710,19 +1710,19 @@
         <v>7022.4000000000005</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44831</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J29" s="4">
@@ -1755,19 +1755,19 @@
         <v>6960.8000000000011</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G30" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44832</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J30" s="4">
@@ -1800,19 +1800,19 @@
         <v>6899.2000000000007</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44833</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J31" s="4">
@@ -1845,19 +1845,19 @@
         <v>6837.6000000000013</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G32" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44834</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J32" s="4">
@@ -1890,19 +1890,19 @@
         <v>6776.0000000000009</v>
       </c>
       <c r="F33" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G33" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44835</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J33" s="4">
@@ -1935,19 +1935,19 @@
         <v>6714.4000000000005</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44836</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J34" s="4">
@@ -1972,7 +1972,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="5"/>
+        <f>D3/2</f>
         <v>61.600000000000009</v>
       </c>
       <c r="E35" s="4">
@@ -1980,19 +1980,19 @@
         <v>3326.4000000000005</v>
       </c>
       <c r="F35" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G35" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44837</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J35" s="4">
@@ -2017,7 +2017,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D36:D38" si="10">D4/2</f>
         <v>61.600000000000009</v>
       </c>
       <c r="E36" s="4">
@@ -2025,19 +2025,19 @@
         <v>3295.6000000000004</v>
       </c>
       <c r="F36" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G36" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44838</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J36" s="4">
@@ -2062,7 +2062,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E37" s="4">
@@ -2070,19 +2070,19 @@
         <v>3264.8000000000006</v>
       </c>
       <c r="F37" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G37" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44839</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J37" s="4">
@@ -2107,7 +2107,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>61.600000000000009</v>
       </c>
       <c r="E38" s="4">
@@ -2115,19 +2115,19 @@
         <v>3234.0000000000005</v>
       </c>
       <c r="F38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="G38" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44840</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J38" s="4">
@@ -2158,7 +2158,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="2">
-        <f>TRUNC(SUM(K3:K38))</f>
+        <f>_xlfn.FLOOR.MATH(SUM(K3:K38))</f>
         <v>262315</v>
       </c>
       <c r="D40" s="3"/>

</xml_diff>

<commit_message>
Update 25. table1 edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB2C70-8989-48E4-9510-E6D3A0369862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FA6A9E-8540-49D1-9837-B415F3F252AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>A$1 * 1.1</f>
+        <f>A1 * 1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -577,7 +577,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D34" si="5">A$1 * 1.1</f>
+        <f>D3</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">
@@ -593,11 +593,11 @@
         <v>44806</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H38" si="6">IF(G4&gt;F4,G4-F4,0)</f>
+        <f t="shared" ref="H4:H38" si="5">IF(G4&gt;F4,G4-F4,0)</f>
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I38" si="7">I3</f>
+        <f t="shared" ref="I4:I38" si="6">I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="4">
@@ -622,7 +622,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D5:D34" si="7">D4</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="4">
@@ -638,11 +638,11 @@
         <v>44807</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J5" s="4">
@@ -667,7 +667,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E6" s="4">
@@ -683,11 +683,11 @@
         <v>44808</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J6" s="4">
@@ -712,7 +712,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E7" s="4">
@@ -728,11 +728,11 @@
         <v>44809</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J7" s="4">
@@ -757,7 +757,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E8" s="4">
@@ -773,11 +773,11 @@
         <v>44810</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J8" s="4">
@@ -802,7 +802,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E9" s="4">
@@ -818,11 +818,11 @@
         <v>44811</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J9" s="4">
@@ -847,7 +847,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E10" s="4">
@@ -863,11 +863,11 @@
         <v>44812</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J10" s="4">
@@ -892,7 +892,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E11" s="4">
@@ -908,11 +908,11 @@
         <v>44813</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J11" s="4">
@@ -937,7 +937,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E12" s="4">
@@ -953,11 +953,11 @@
         <v>44814</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J12" s="4">
@@ -982,7 +982,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E13" s="4">
@@ -998,11 +998,11 @@
         <v>44815</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J13" s="4">
@@ -1027,7 +1027,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E14" s="4">
@@ -1043,11 +1043,11 @@
         <v>44816</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J14" s="4">
@@ -1072,7 +1072,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E15" s="4">
@@ -1088,11 +1088,11 @@
         <v>44817</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J15" s="4">
@@ -1117,7 +1117,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E16" s="4">
@@ -1133,11 +1133,11 @@
         <v>44818</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J16" s="4">
@@ -1162,7 +1162,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E17" s="4">
@@ -1178,11 +1178,11 @@
         <v>44819</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J17" s="4">
@@ -1207,7 +1207,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E18" s="4">
@@ -1223,11 +1223,11 @@
         <v>44820</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J18" s="4">
@@ -1252,7 +1252,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E19" s="4">
@@ -1268,11 +1268,11 @@
         <v>44821</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J19" s="4">
@@ -1297,7 +1297,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E20" s="4">
@@ -1313,11 +1313,11 @@
         <v>44822</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J20" s="4">
@@ -1342,7 +1342,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E21" s="4">
@@ -1358,11 +1358,11 @@
         <v>44823</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J21" s="4">
@@ -1387,7 +1387,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E22" s="4">
@@ -1403,11 +1403,11 @@
         <v>44824</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J22" s="4">
@@ -1432,7 +1432,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E23" s="4">
@@ -1448,11 +1448,11 @@
         <v>44825</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J23" s="4">
@@ -1477,7 +1477,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E24" s="4">
@@ -1493,11 +1493,11 @@
         <v>44826</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J24" s="4">
@@ -1522,7 +1522,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E25" s="4">
@@ -1538,11 +1538,11 @@
         <v>44827</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J25" s="4">
@@ -1567,7 +1567,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E26" s="4">
@@ -1583,11 +1583,11 @@
         <v>44828</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J26" s="4">
@@ -1612,7 +1612,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E27" s="4">
@@ -1628,11 +1628,11 @@
         <v>44829</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J27" s="4">
@@ -1657,7 +1657,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E28" s="4">
@@ -1673,11 +1673,11 @@
         <v>44830</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J28" s="4">
@@ -1702,7 +1702,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E29" s="4">
@@ -1718,11 +1718,11 @@
         <v>44831</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J29" s="4">
@@ -1747,7 +1747,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E30" s="4">
@@ -1763,11 +1763,11 @@
         <v>44832</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J30" s="4">
@@ -1792,7 +1792,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E31" s="4">
@@ -1808,11 +1808,11 @@
         <v>44833</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J31" s="4">
@@ -1837,7 +1837,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E32" s="4">
@@ -1853,11 +1853,11 @@
         <v>44834</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J32" s="4">
@@ -1882,7 +1882,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E33" s="4">
@@ -1898,11 +1898,11 @@
         <v>44835</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J33" s="4">
@@ -1927,7 +1927,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E34" s="4">
@@ -1943,11 +1943,11 @@
         <v>44836</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J34" s="4">
@@ -1988,11 +1988,11 @@
         <v>44837</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J35" s="4">
@@ -2033,11 +2033,11 @@
         <v>44838</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J36" s="4">
@@ -2078,11 +2078,11 @@
         <v>44839</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J37" s="4">
@@ -2123,11 +2123,11 @@
         <v>44840</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J38" s="4">
@@ -2158,7 +2158,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="2">
-        <f>_xlfn.FLOOR.MATH(SUM(K3:K38))</f>
+        <f>FLOOR(SUM(K3:K38),1)</f>
         <v>262315</v>
       </c>
       <c r="D40" s="3"/>
@@ -2227,5 +2227,8 @@
   </sheetData>
   <pageMargins left="0.70000004768371604" right="0.70000004768371604" top="0.75" bottom="0.75" header="0.30000001192092901" footer="0.30000001192092901"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E4" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update 26. table1 edited
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD91F91-F8BD-4A3E-8A87-F4228DB6D798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5043822-0D81-4F99-96A9-49BB10700038}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="4">
-        <f>A1*1.1</f>
+        <f>A$1*1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E3" s="4">
@@ -576,7 +576,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="4">
-        <f>IF(A3+1&lt;33,D$3,D$3*0.5)</f>
+        <f t="shared" ref="D4:D34" si="5">A$1*1.1</f>
         <v>123.20000000000002</v>
       </c>
       <c r="E4" s="4">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I38" si="5">I3</f>
+        <f t="shared" ref="I4:I38" si="6">I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="4">
@@ -621,7 +621,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D38" si="6">IF(A4+1&lt;33,D$3,D$3*0.5)</f>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E5" s="4">
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J5" s="4">
@@ -666,7 +666,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E6" s="4">
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J6" s="4">
@@ -711,7 +711,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E7" s="4">
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J7" s="4">
@@ -756,7 +756,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E8" s="4">
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J8" s="4">
@@ -801,7 +801,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E9" s="4">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J9" s="4">
@@ -846,7 +846,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E10" s="4">
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J10" s="4">
@@ -891,7 +891,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E11" s="4">
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J11" s="4">
@@ -936,7 +936,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E12" s="4">
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J12" s="4">
@@ -981,7 +981,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E13" s="4">
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J13" s="4">
@@ -1026,7 +1026,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E14" s="4">
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J14" s="4">
@@ -1071,7 +1071,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E15" s="4">
@@ -1091,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J15" s="4">
@@ -1116,7 +1116,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E16" s="4">
@@ -1136,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J16" s="4">
@@ -1161,7 +1161,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E17" s="4">
@@ -1181,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J17" s="4">
@@ -1206,7 +1206,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E18" s="4">
@@ -1226,7 +1226,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J18" s="4">
@@ -1251,7 +1251,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E19" s="4">
@@ -1271,7 +1271,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J19" s="4">
@@ -1296,7 +1296,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E20" s="4">
@@ -1316,7 +1316,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J20" s="4">
@@ -1341,7 +1341,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E21" s="4">
@@ -1361,7 +1361,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J21" s="4">
@@ -1386,7 +1386,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E22" s="4">
@@ -1406,7 +1406,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J22" s="4">
@@ -1431,7 +1431,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E23" s="4">
@@ -1451,7 +1451,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J23" s="4">
@@ -1476,7 +1476,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E24" s="4">
@@ -1496,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J24" s="4">
@@ -1521,7 +1521,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E25" s="4">
@@ -1541,7 +1541,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J25" s="4">
@@ -1566,7 +1566,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E26" s="4">
@@ -1586,7 +1586,7 @@
         <v>15</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J26" s="4">
@@ -1611,7 +1611,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E27" s="4">
@@ -1631,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J27" s="4">
@@ -1656,7 +1656,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E28" s="4">
@@ -1676,7 +1676,7 @@
         <v>17</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J28" s="4">
@@ -1701,7 +1701,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E29" s="4">
@@ -1721,7 +1721,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J29" s="4">
@@ -1746,7 +1746,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E30" s="4">
@@ -1766,7 +1766,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J30" s="4">
@@ -1791,7 +1791,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E31" s="4">
@@ -1811,7 +1811,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J31" s="4">
@@ -1836,7 +1836,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E32" s="4">
@@ -1856,7 +1856,7 @@
         <v>21</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J32" s="4">
@@ -1881,7 +1881,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E33" s="4">
@@ -1901,7 +1901,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J33" s="4">
@@ -1926,7 +1926,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
       <c r="E34" s="4">
@@ -1946,7 +1946,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J34" s="4">
@@ -1971,12 +1971,12 @@
         <v>54</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="6"/>
-        <v>61.600000000000009</v>
+        <f>D3/3</f>
+        <v>41.06666666666667</v>
       </c>
       <c r="E35" s="4">
         <f t="shared" si="0"/>
-        <v>3326.4000000000005</v>
+        <v>2217.6000000000004</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" si="7"/>
@@ -1991,7 +1991,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J35" s="4">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="K35" s="4">
         <f t="shared" si="2"/>
-        <v>3566.4000000000005</v>
+        <v>2457.6000000000004</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2016,12 +2016,12 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="6"/>
-        <v>61.600000000000009</v>
+        <f t="shared" ref="D36:D38" si="10">D4/3</f>
+        <v>41.06666666666667</v>
       </c>
       <c r="E36" s="4">
         <f t="shared" si="0"/>
-        <v>3295.6000000000004</v>
+        <v>2197.0666666666671</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" si="7"/>
@@ -2036,7 +2036,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J36" s="4">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="K36" s="4">
         <f t="shared" si="2"/>
-        <v>3545.6000000000004</v>
+        <v>2447.0666666666671</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2061,12 +2061,12 @@
         <v>53</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="6"/>
-        <v>61.600000000000009</v>
+        <f t="shared" si="10"/>
+        <v>41.06666666666667</v>
       </c>
       <c r="E37" s="4">
         <f t="shared" si="0"/>
-        <v>3264.8000000000006</v>
+        <v>2176.5333333333333</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="7"/>
@@ -2081,7 +2081,7 @@
         <v>26</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J37" s="4">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="K37" s="4">
         <f t="shared" si="2"/>
-        <v>3524.8000000000006</v>
+        <v>2436.5333333333333</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2106,12 +2106,12 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="6"/>
-        <v>61.600000000000009</v>
+        <f t="shared" si="10"/>
+        <v>41.06666666666667</v>
       </c>
       <c r="E38" s="4">
         <f t="shared" si="0"/>
-        <v>3234.0000000000005</v>
+        <v>2156</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" si="7"/>
@@ -2126,7 +2126,7 @@
         <v>27</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J38" s="4">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="K38" s="4">
         <f t="shared" si="2"/>
-        <v>3504.0000000000005</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="C40" s="2">
         <f>TRUNC(SUM(K3:K38))</f>
-        <v>262315</v>
+        <v>257941</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>

</xml_diff>

<commit_message>
Update ??. edited table_1_112
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\LR3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A331DE8A-E76C-4521-83B1-8CA177224353}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28830" windowHeight="12765"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -178,8 +172,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +183,8 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -452,14 +448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="1" customWidth="1"/>
@@ -474,7 +470,7 @@
     <col min="11" max="11" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="4">
         <v>112</v>
       </c>
@@ -489,7 +485,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -524,7 +520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -564,7 +560,7 @@
         <v>8624.0000000000018</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A38" si="3">A3+1</f>
         <v>2</v>
@@ -609,7 +605,7 @@
         <v>8562.4000000000015</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="2">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -654,7 +650,7 @@
         <v>8500.8000000000011</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="2">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -699,7 +695,7 @@
         <v>8439.2000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="2">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -744,7 +740,7 @@
         <v>8377.6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75">
       <c r="A8" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -789,7 +785,7 @@
         <v>8316.0000000000018</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75">
       <c r="A9" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -834,7 +830,7 @@
         <v>8254.4000000000015</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75">
       <c r="A10" s="2">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -879,7 +875,7 @@
         <v>8192.8000000000011</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75">
       <c r="A11" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -924,7 +920,7 @@
         <v>8131.2000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75">
       <c r="A12" s="2">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -969,7 +965,7 @@
         <v>8079.6000000000013</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="2">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1014,7 +1010,7 @@
         <v>8028.0000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="2">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1059,7 +1055,7 @@
         <v>7976.4000000000015</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="2">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1104,7 +1100,7 @@
         <v>7924.8000000000011</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -1149,7 +1145,7 @@
         <v>7873.2000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75">
       <c r="A17" s="2">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -1194,7 +1190,7 @@
         <v>7821.6000000000013</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.75">
       <c r="A18" s="2">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -1239,7 +1235,7 @@
         <v>7770.0000000000009</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="2">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -1284,7 +1280,7 @@
         <v>7718.4000000000015</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75">
       <c r="A20" s="2">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -1329,7 +1325,7 @@
         <v>7666.8000000000011</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75">
       <c r="A21" s="2">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -1374,7 +1370,7 @@
         <v>7615.2000000000007</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75">
       <c r="A22" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -1419,7 +1415,7 @@
         <v>7563.6000000000013</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75">
       <c r="A23" s="2">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -1464,7 +1460,7 @@
         <v>7512.0000000000009</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.75">
       <c r="A24" s="2">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -1509,7 +1505,7 @@
         <v>7460.4000000000015</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75">
       <c r="A25" s="2">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -1554,7 +1550,7 @@
         <v>7408.8000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75">
       <c r="A26" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -1599,7 +1595,7 @@
         <v>7357.2000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75">
       <c r="A27" s="2">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -1644,7 +1640,7 @@
         <v>7305.6000000000013</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75">
       <c r="A28" s="2">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -1689,7 +1685,7 @@
         <v>7254.0000000000009</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="2">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -1734,7 +1730,7 @@
         <v>7202.4000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15.75">
       <c r="A30" s="2">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -1779,7 +1775,7 @@
         <v>7150.8000000000011</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15.75">
       <c r="A31" s="2">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -1824,7 +1820,7 @@
         <v>7099.2000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15.75">
       <c r="A32" s="2">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -1869,7 +1865,7 @@
         <v>7047.6000000000013</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15.75">
       <c r="A33" s="2">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -1914,7 +1910,7 @@
         <v>6996.0000000000009</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15.75">
       <c r="A34" s="2">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -1959,7 +1955,7 @@
         <v>6944.4000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15.75">
       <c r="A35" s="2">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -2004,7 +2000,7 @@
         <v>3566.4000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15.75">
       <c r="A36" s="2">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -2049,7 +2045,7 @@
         <v>3545.6000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15.75">
       <c r="A37" s="2">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -2094,7 +2090,7 @@
         <v>3524.8000000000006</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15.75">
       <c r="A38" s="2">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -2139,7 +2135,7 @@
         <v>3504.0000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.75">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2152,13 +2148,13 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15.75">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="2">
-        <f>TRUNC(SUM(K3:K38))</f>
+        <f>FLOOR(SUM(K3:K38), 1)</f>
         <v>262315</v>
       </c>
       <c r="D40" s="3"/>
@@ -2170,7 +2166,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15.75">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
         <v>46</v>
@@ -2188,7 +2184,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15.75">
       <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
         <v>47</v>
@@ -2206,7 +2202,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15.75">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Update 2. edited table_1_112
</commit_message>
<xml_diff>
--- a/LR3/table_1_112.xlsx
+++ b/LR3/table_1_112.xlsx
@@ -451,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -2154,7 +2154,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="2">
-        <f>FLOOR(SUM(K3:K38), 1)</f>
+        <f>FLOOR(SUM(K3:K38),1)</f>
         <v>262315</v>
       </c>
       <c r="D40" s="3"/>

</xml_diff>